<commit_message>
Fixed bug in Marescoe-David query corpus script
</commit_message>
<xml_diff>
--- a/datasets/annotated_dataset_marescoe-david.xlsx
+++ b/datasets/annotated_dataset_marescoe-david.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenvansweeveldt/Documents/Universiteit/Thesis/github/DTA_Thesis/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BFEEAD-52F7-AE4B-AE2B-58B12D316014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D08BA6-D6EC-E747-8082-01F80A7BE9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="520" windowWidth="26040" windowHeight="15900" xr2:uid="{2DE8A2F7-5C91-7244-8471-433F9B1E60CC}"/>
+    <workbookView xWindow="5360" yWindow="1080" windowWidth="26040" windowHeight="15900" xr2:uid="{2DE8A2F7-5C91-7244-8471-433F9B1E60CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6674,19 +6674,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6705,6 +6692,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6769,37 +6769,37 @@
     <sortCondition ref="S1:S420"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{2B274604-1AB0-474D-BC18-DA231FB86FE3}" name="NR" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{5F5758D9-D68B-A94F-ABDA-B520067D2B89}" name="SENDER" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{6B408867-D8BB-EC43-978C-AE22D22CF317}" name="ADDRESSEE" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{6FB1564F-5499-D041-9B9D-D2EF34C2E3FA}" name="SENDER-ADDRESSEE_PAIRS" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{55FF3603-1D69-D244-8A62-CBD7E0E933C2}" name="DATE" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{C9BE50B2-2E91-884D-BB24-789B01C25B7F}" name="YEAR" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{E227D5BF-CF2D-3945-BACF-F864EA55DF0E}" name="LANGUAGE" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{5EF9593C-ED83-A643-BA80-767152BA8574}" name="GENDER_SENDER" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{AAAE1B88-5BB9-6E4F-910A-D544E0979D75}" name="GENDER_ADDRESSEE" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{6297521E-720B-4445-9BD8-12D9AD45225A}" name="GENDER_PAIR" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{89746025-7DB7-A04A-9541-7D46C6030F98}" name="CONNECTION_TYPE" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{2F1D5254-C06E-444E-97C6-FC8CA77A4F2B}" name="GENERATION_SENDER" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{86481F33-84C3-174C-9F28-8D0E24322839}" name="GENERATION_ADDRESSEE" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{C181A9FE-74D7-9449-A3A2-2AD0178B3B7A}" name="SENDER_IS_OLDER" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{6EFC6140-457F-8442-808A-F76D1AFF06ED}" name="SENDER_OVER_40" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{FEA81B60-3DDD-7548-90B0-96B78A01FAC1}" name="ADDRESSEE_OVER_40" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{8D7094B5-69C2-3848-B7A8-D097AA8FE8DC}" name="AGE_GAP_OVER_20" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{6A946987-1263-B445-BDFA-2FDE2CC7B594}" name="AGE_GAP" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{C582C7E0-7EC6-5047-9B60-C576DCFD7566}" name="PAGE" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{0427B90F-9B1D-3540-9FC1-920DB3A87387}" name="LENGTH" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{F605F5C0-EFF3-CC4A-84F0-7AB6C3A39330}" name="TOKEN_ID" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{D9F44558-DA44-DD43-A055-DFC7AD9E4A42}" name="REL_TOKEN_POS" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{0BC612CA-6C79-1447-AE28-BE2B21DCD776}" name="QUERY" dataDxfId="3"/>
-    <tableColumn id="24" xr3:uid="{B7C67CE6-590D-6542-B95D-C4C6D6F658C6}" name="LEFT" dataDxfId="2"/>
-    <tableColumn id="25" xr3:uid="{F9652450-1444-5742-A437-939FC87EF739}" name="HIT" dataDxfId="1"/>
-    <tableColumn id="26" xr3:uid="{33EC8E1C-842D-AA4C-9494-236E178DCBDB}" name="RIGHT" dataDxfId="0"/>
-    <tableColumn id="27" xr3:uid="{987E508C-0103-AC4A-8D66-52F6C036AB5F}" name="LABEL" dataDxfId="30"/>
-    <tableColumn id="28" xr3:uid="{3657F2E6-B20E-CB49-9995-538B3EF00FE4}" name="DOMAIN" dataDxfId="29"/>
-    <tableColumn id="29" xr3:uid="{DB1C4657-865F-0247-9AF9-7AF6DB2A80E7}" name="FORMULA_TYPE" dataDxfId="28"/>
-    <tableColumn id="30" xr3:uid="{D0BBCF8A-E85F-4A48-8952-DDA504B5CFCE}" name="FORMULA" dataDxfId="27"/>
-    <tableColumn id="31" xr3:uid="{8B5B0594-0A86-C144-81AD-0ED57FB6AA37}" name="NOTE" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{2B274604-1AB0-474D-BC18-DA231FB86FE3}" name="NR" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{5F5758D9-D68B-A94F-ABDA-B520067D2B89}" name="SENDER" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{6B408867-D8BB-EC43-978C-AE22D22CF317}" name="ADDRESSEE" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{6FB1564F-5499-D041-9B9D-D2EF34C2E3FA}" name="SENDER-ADDRESSEE_PAIRS" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{55FF3603-1D69-D244-8A62-CBD7E0E933C2}" name="DATE" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C9BE50B2-2E91-884D-BB24-789B01C25B7F}" name="YEAR" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{E227D5BF-CF2D-3945-BACF-F864EA55DF0E}" name="LANGUAGE" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{5EF9593C-ED83-A643-BA80-767152BA8574}" name="GENDER_SENDER" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{AAAE1B88-5BB9-6E4F-910A-D544E0979D75}" name="GENDER_ADDRESSEE" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{6297521E-720B-4445-9BD8-12D9AD45225A}" name="GENDER_PAIR" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{89746025-7DB7-A04A-9541-7D46C6030F98}" name="CONNECTION_TYPE" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{2F1D5254-C06E-444E-97C6-FC8CA77A4F2B}" name="GENERATION_SENDER" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{86481F33-84C3-174C-9F28-8D0E24322839}" name="GENERATION_ADDRESSEE" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{C181A9FE-74D7-9449-A3A2-2AD0178B3B7A}" name="SENDER_IS_OLDER" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{6EFC6140-457F-8442-808A-F76D1AFF06ED}" name="SENDER_OVER_40" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{FEA81B60-3DDD-7548-90B0-96B78A01FAC1}" name="ADDRESSEE_OVER_40" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{8D7094B5-69C2-3848-B7A8-D097AA8FE8DC}" name="AGE_GAP_OVER_20" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{6A946987-1263-B445-BDFA-2FDE2CC7B594}" name="AGE_GAP" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{C582C7E0-7EC6-5047-9B60-C576DCFD7566}" name="PAGE" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{0427B90F-9B1D-3540-9FC1-920DB3A87387}" name="LENGTH" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{F605F5C0-EFF3-CC4A-84F0-7AB6C3A39330}" name="TOKEN_ID" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{D9F44558-DA44-DD43-A055-DFC7AD9E4A42}" name="REL_TOKEN_POS" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{0BC612CA-6C79-1447-AE28-BE2B21DCD776}" name="QUERY" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{B7C67CE6-590D-6542-B95D-C4C6D6F658C6}" name="LEFT" dataDxfId="8"/>
+    <tableColumn id="25" xr3:uid="{F9652450-1444-5742-A437-939FC87EF739}" name="HIT" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{33EC8E1C-842D-AA4C-9494-236E178DCBDB}" name="RIGHT" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{987E508C-0103-AC4A-8D66-52F6C036AB5F}" name="LABEL" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{3657F2E6-B20E-CB49-9995-538B3EF00FE4}" name="DOMAIN" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{DB1C4657-865F-0247-9AF9-7AF6DB2A80E7}" name="FORMULA_TYPE" dataDxfId="3"/>
+    <tableColumn id="30" xr3:uid="{D0BBCF8A-E85F-4A48-8952-DDA504B5CFCE}" name="FORMULA" dataDxfId="2"/>
+    <tableColumn id="31" xr3:uid="{8B5B0594-0A86-C144-81AD-0ED57FB6AA37}" name="NOTE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7104,8 +7104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701675D7-A1E8-FE4D-8037-276CD2CD5302}">
   <dimension ref="A1:AE420"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="D405" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E416" sqref="E416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7255,6 +7255,9 @@
       <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F2" s="1">
+        <v>1667</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
@@ -7341,6 +7344,9 @@
       <c r="E3" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="F3" s="1">
+        <v>1668</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
@@ -7430,6 +7436,9 @@
       <c r="E4" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="F4" s="1">
+        <v>1668</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
@@ -7519,6 +7528,9 @@
       <c r="E5" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="F5" s="1">
+        <v>1668</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>46</v>
       </c>
@@ -7608,6 +7620,9 @@
       <c r="E6" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F6" s="1">
+        <v>1668</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
@@ -7700,6 +7715,9 @@
       <c r="E7" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="F7" s="1">
+        <v>1668</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>46</v>
       </c>
@@ -7792,6 +7810,9 @@
       <c r="E8" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="F8" s="1">
+        <v>1668</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>85</v>
       </c>
@@ -7884,6 +7905,9 @@
       <c r="E9" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="F9" s="1">
+        <v>1668</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>85</v>
       </c>
@@ -7973,6 +7997,9 @@
       <c r="E10" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="F10" s="1">
+        <v>1668</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>46</v>
       </c>
@@ -8059,6 +8086,9 @@
       <c r="E11" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="F11" s="1">
+        <v>1668</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>46</v>
       </c>
@@ -8145,6 +8175,9 @@
       <c r="E12" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="F12" s="1">
+        <v>1668</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>46</v>
       </c>
@@ -8231,6 +8264,9 @@
       <c r="E13" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="F13" s="1">
+        <v>1668</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>85</v>
       </c>
@@ -8320,6 +8356,9 @@
       <c r="E14" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="F14" s="1">
+        <v>1668</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>46</v>
       </c>
@@ -8409,6 +8448,9 @@
       <c r="E15" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="F15" s="1">
+        <v>1668</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>31</v>
       </c>
@@ -8486,6 +8528,9 @@
       <c r="E16" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="F16" s="1">
+        <v>1668</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>31</v>
       </c>
@@ -8575,6 +8620,9 @@
       <c r="E17" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F17" s="1">
+        <v>1668</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>46</v>
       </c>
@@ -8664,6 +8712,9 @@
       <c r="E18" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F18" s="1">
+        <v>1668</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -8753,6 +8804,9 @@
       <c r="E19" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F19" s="1">
+        <v>1668</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
@@ -8842,6 +8896,9 @@
       <c r="E20" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F20" s="1">
+        <v>1668</v>
+      </c>
       <c r="G20" s="1" t="s">
         <v>46</v>
       </c>
@@ -8931,6 +8988,9 @@
       <c r="E21" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F21" s="1">
+        <v>1668</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>46</v>
       </c>
@@ -9020,6 +9080,9 @@
       <c r="E22" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F22" s="1">
+        <v>1668</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>46</v>
       </c>
@@ -9109,6 +9172,9 @@
       <c r="E23" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F23" s="1">
+        <v>1668</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>46</v>
       </c>
@@ -9198,6 +9264,9 @@
       <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="F24" s="1">
+        <v>1668</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>85</v>
       </c>
@@ -9290,6 +9359,9 @@
       <c r="E25" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="F25" s="1">
+        <v>1668</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>85</v>
       </c>
@@ -9382,6 +9454,9 @@
       <c r="E26" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="F26" s="1">
+        <v>1668</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>46</v>
       </c>
@@ -9468,6 +9543,9 @@
       <c r="E27" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="F27" s="1">
+        <v>1668</v>
+      </c>
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
@@ -9554,6 +9632,9 @@
       <c r="E28" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="F28" s="1">
+        <v>1668</v>
+      </c>
       <c r="G28" s="1" t="s">
         <v>46</v>
       </c>
@@ -9640,6 +9721,9 @@
       <c r="E29" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="F29" s="1">
+        <v>1668</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>46</v>
       </c>
@@ -9717,6 +9801,9 @@
       <c r="E30" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="F30" s="1">
+        <v>1668</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>46</v>
       </c>
@@ -9803,6 +9890,9 @@
       <c r="E31" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="F31" s="1">
+        <v>1668</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>46</v>
       </c>
@@ -9889,6 +9979,9 @@
       <c r="E32" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="F32" s="1">
+        <v>1668</v>
+      </c>
       <c r="G32" s="1" t="s">
         <v>46</v>
       </c>
@@ -9978,6 +10071,9 @@
       <c r="E33" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="F33" s="1">
+        <v>1668</v>
+      </c>
       <c r="G33" s="1" t="s">
         <v>46</v>
       </c>
@@ -10067,6 +10163,9 @@
       <c r="E34" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="F34" s="1">
+        <v>1668</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>46</v>
       </c>
@@ -10153,6 +10252,9 @@
       <c r="E35" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="F35" s="1">
+        <v>1668</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>31</v>
       </c>
@@ -10233,6 +10335,9 @@
       <c r="E36" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="F36" s="1">
+        <v>1668</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>31</v>
       </c>
@@ -10313,6 +10418,9 @@
       <c r="E37" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="F37" s="1">
+        <v>1668</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>31</v>
       </c>
@@ -10393,6 +10501,9 @@
       <c r="E38" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="F38" s="1">
+        <v>1668</v>
+      </c>
       <c r="G38" s="1" t="s">
         <v>31</v>
       </c>
@@ -10633,6 +10744,9 @@
       <c r="E41" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="F41" s="1">
+        <v>1668</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>31</v>
       </c>
@@ -10713,6 +10827,9 @@
       <c r="E42" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="F42" s="1">
+        <v>1668</v>
+      </c>
       <c r="G42" s="1" t="s">
         <v>31</v>
       </c>
@@ -10790,6 +10907,9 @@
       <c r="E43" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="F43" s="1">
+        <v>1668</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>46</v>
       </c>
@@ -10876,6 +10996,9 @@
       <c r="E44" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="F44" s="1">
+        <v>1668</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>46</v>
       </c>
@@ -10965,6 +11088,9 @@
       <c r="E45" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="F45" s="1">
+        <v>1668</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>46</v>
       </c>
@@ -11051,6 +11177,9 @@
       <c r="E46" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="F46" s="1">
+        <v>1668</v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>46</v>
       </c>
@@ -11128,6 +11257,9 @@
       <c r="E47" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="F47" s="1">
+        <v>1668</v>
+      </c>
       <c r="G47" s="1" t="s">
         <v>46</v>
       </c>
@@ -11205,6 +11337,9 @@
       <c r="E48" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="F48" s="1">
+        <v>1668</v>
+      </c>
       <c r="G48" s="1" t="s">
         <v>46</v>
       </c>
@@ -11291,6 +11426,9 @@
       <c r="E49" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="F49" s="1">
+        <v>1668</v>
+      </c>
       <c r="G49" s="1" t="s">
         <v>46</v>
       </c>
@@ -11377,6 +11515,9 @@
       <c r="E50" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="F50" s="1">
+        <v>1668</v>
+      </c>
       <c r="G50" s="1" t="s">
         <v>46</v>
       </c>
@@ -11466,6 +11607,9 @@
       <c r="E51" s="1" t="s">
         <v>291</v>
       </c>
+      <c r="F51" s="1">
+        <v>1668</v>
+      </c>
       <c r="G51" s="1" t="s">
         <v>31</v>
       </c>
@@ -11552,6 +11696,9 @@
       <c r="E52" s="1" t="s">
         <v>298</v>
       </c>
+      <c r="F52" s="1">
+        <v>1668</v>
+      </c>
       <c r="G52" s="1" t="s">
         <v>46</v>
       </c>
@@ -11641,6 +11788,9 @@
       <c r="E53" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="F53" s="1">
+        <v>1669</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>31</v>
       </c>
@@ -11721,6 +11871,9 @@
       <c r="E54" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="F54" s="1">
+        <v>1668</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>46</v>
       </c>
@@ -11813,6 +11966,9 @@
       <c r="E55" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="F55" s="1">
+        <v>1669</v>
+      </c>
       <c r="G55" s="1" t="s">
         <v>31</v>
       </c>
@@ -11893,6 +12049,9 @@
       <c r="E56" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="F56" s="1">
+        <v>1668</v>
+      </c>
       <c r="G56" s="1" t="s">
         <v>46</v>
       </c>
@@ -11973,6 +12132,9 @@
       <c r="E57" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="F57" s="1">
+        <v>1668</v>
+      </c>
       <c r="G57" s="1" t="s">
         <v>46</v>
       </c>
@@ -12062,6 +12224,9 @@
       <c r="E58" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="F58" s="1">
+        <v>1668</v>
+      </c>
       <c r="G58" s="1" t="s">
         <v>46</v>
       </c>
@@ -12148,6 +12313,9 @@
       <c r="E59" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="F59" s="1">
+        <v>1668</v>
+      </c>
       <c r="G59" s="1" t="s">
         <v>46</v>
       </c>
@@ -12225,6 +12393,9 @@
       <c r="E60" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="F60" s="1">
+        <v>1668</v>
+      </c>
       <c r="G60" s="1" t="s">
         <v>46</v>
       </c>
@@ -12314,6 +12485,9 @@
       <c r="E61" s="1" t="s">
         <v>338</v>
       </c>
+      <c r="F61" s="1">
+        <v>1669</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>85</v>
       </c>
@@ -12400,6 +12574,9 @@
       <c r="E62" s="1" t="s">
         <v>343</v>
       </c>
+      <c r="F62" s="1">
+        <v>1669</v>
+      </c>
       <c r="G62" s="1" t="s">
         <v>85</v>
       </c>
@@ -12480,6 +12657,9 @@
       <c r="E63" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="F63" s="1">
+        <v>1668</v>
+      </c>
       <c r="G63" s="1" t="s">
         <v>46</v>
       </c>
@@ -12569,6 +12749,9 @@
       <c r="E64" s="1" t="s">
         <v>355</v>
       </c>
+      <c r="F64" s="1">
+        <v>1669</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>31</v>
       </c>
@@ -12646,6 +12829,9 @@
       <c r="E65" s="1" t="s">
         <v>364</v>
       </c>
+      <c r="F65" s="1">
+        <v>1669</v>
+      </c>
       <c r="G65" s="1" t="s">
         <v>46</v>
       </c>
@@ -12729,6 +12915,9 @@
       <c r="E66" s="1" t="s">
         <v>364</v>
       </c>
+      <c r="F66" s="1">
+        <v>1669</v>
+      </c>
       <c r="G66" s="1" t="s">
         <v>46</v>
       </c>
@@ -12815,6 +13004,9 @@
       <c r="E67" s="1" t="s">
         <v>373</v>
       </c>
+      <c r="F67" s="1">
+        <v>1669</v>
+      </c>
       <c r="G67" s="1" t="s">
         <v>46</v>
       </c>
@@ -12904,6 +13096,9 @@
       <c r="E68" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="F68" s="1">
+        <v>1669</v>
+      </c>
       <c r="G68" s="1" t="s">
         <v>46</v>
       </c>
@@ -12990,6 +13185,9 @@
       <c r="E69" s="1" t="s">
         <v>385</v>
       </c>
+      <c r="F69" s="1">
+        <v>1669</v>
+      </c>
       <c r="G69" s="1" t="s">
         <v>46</v>
       </c>
@@ -13082,6 +13280,9 @@
       <c r="E70" s="1" t="s">
         <v>385</v>
       </c>
+      <c r="F70" s="1">
+        <v>1669</v>
+      </c>
       <c r="G70" s="1" t="s">
         <v>46</v>
       </c>
@@ -13171,6 +13372,9 @@
       <c r="E71" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="F71" s="1">
+        <v>1669</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>46</v>
       </c>
@@ -13257,6 +13461,9 @@
       <c r="E72" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="F72" s="1">
+        <v>1669</v>
+      </c>
       <c r="G72" s="1" t="s">
         <v>46</v>
       </c>
@@ -13343,6 +13550,9 @@
       <c r="E73" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="F73" s="1">
+        <v>1669</v>
+      </c>
       <c r="G73" s="1" t="s">
         <v>46</v>
       </c>
@@ -13429,6 +13639,9 @@
       <c r="E74" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="F74" s="1">
+        <v>1669</v>
+      </c>
       <c r="G74" s="1" t="s">
         <v>46</v>
       </c>
@@ -13515,6 +13728,9 @@
       <c r="E75" s="1" t="s">
         <v>411</v>
       </c>
+      <c r="F75" s="1">
+        <v>1669</v>
+      </c>
       <c r="G75" s="1" t="s">
         <v>31</v>
       </c>
@@ -13607,6 +13823,9 @@
       <c r="E76" s="1" t="s">
         <v>411</v>
       </c>
+      <c r="F76" s="1">
+        <v>1669</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>31</v>
       </c>
@@ -13687,6 +13906,9 @@
       <c r="E77" s="1" t="s">
         <v>411</v>
       </c>
+      <c r="F77" s="1">
+        <v>1669</v>
+      </c>
       <c r="G77" s="1" t="s">
         <v>31</v>
       </c>
@@ -13764,6 +13986,9 @@
       <c r="E78" s="1" t="s">
         <v>422</v>
       </c>
+      <c r="F78" s="1">
+        <v>1669</v>
+      </c>
       <c r="G78" s="1" t="s">
         <v>46</v>
       </c>
@@ -13850,6 +14075,9 @@
       <c r="E79" s="1" t="s">
         <v>427</v>
       </c>
+      <c r="F79" s="1">
+        <v>1669</v>
+      </c>
       <c r="G79" s="1" t="s">
         <v>46</v>
       </c>
@@ -13936,6 +14164,9 @@
       <c r="E80" s="1" t="s">
         <v>427</v>
       </c>
+      <c r="F80" s="1">
+        <v>1669</v>
+      </c>
       <c r="G80" s="1" t="s">
         <v>46</v>
       </c>
@@ -14022,6 +14253,9 @@
       <c r="E81" s="1" t="s">
         <v>427</v>
       </c>
+      <c r="F81" s="1">
+        <v>1669</v>
+      </c>
       <c r="G81" s="1" t="s">
         <v>46</v>
       </c>
@@ -14105,6 +14339,9 @@
       <c r="E82" s="1" t="s">
         <v>427</v>
       </c>
+      <c r="F82" s="1">
+        <v>1669</v>
+      </c>
       <c r="G82" s="1" t="s">
         <v>46</v>
       </c>
@@ -14191,6 +14428,9 @@
       <c r="E83" s="1" t="s">
         <v>441</v>
       </c>
+      <c r="F83" s="1">
+        <v>1669</v>
+      </c>
       <c r="G83" s="1" t="s">
         <v>46</v>
       </c>
@@ -14280,6 +14520,9 @@
       <c r="E84" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="F84" s="1">
+        <v>1669</v>
+      </c>
       <c r="G84" s="1" t="s">
         <v>46</v>
       </c>
@@ -14357,6 +14600,9 @@
       <c r="E85" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="F85" s="1">
+        <v>1669</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>46</v>
       </c>
@@ -14443,6 +14689,9 @@
       <c r="E86" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="F86" s="1">
+        <v>1669</v>
+      </c>
       <c r="G86" s="1" t="s">
         <v>46</v>
       </c>
@@ -14529,6 +14778,9 @@
       <c r="E87" s="1" t="s">
         <v>459</v>
       </c>
+      <c r="F87" s="1">
+        <v>1669</v>
+      </c>
       <c r="G87" s="1" t="s">
         <v>46</v>
       </c>
@@ -14618,6 +14870,9 @@
       <c r="E88" s="1" t="s">
         <v>459</v>
       </c>
+      <c r="F88" s="1">
+        <v>1669</v>
+      </c>
       <c r="G88" s="1" t="s">
         <v>46</v>
       </c>
@@ -14707,6 +14962,9 @@
       <c r="E89" s="1" t="s">
         <v>459</v>
       </c>
+      <c r="F89" s="1">
+        <v>1669</v>
+      </c>
       <c r="G89" s="1" t="s">
         <v>46</v>
       </c>
@@ -14790,6 +15048,9 @@
       <c r="E90" s="1" t="s">
         <v>470</v>
       </c>
+      <c r="F90" s="1">
+        <v>1669</v>
+      </c>
       <c r="G90" s="1" t="s">
         <v>31</v>
       </c>
@@ -14876,6 +15137,9 @@
       <c r="E91" s="1" t="s">
         <v>475</v>
       </c>
+      <c r="F91" s="1">
+        <v>1669</v>
+      </c>
       <c r="G91" s="1" t="s">
         <v>46</v>
       </c>
@@ -14956,6 +15220,9 @@
       <c r="E92" s="1" t="s">
         <v>475</v>
       </c>
+      <c r="F92" s="1">
+        <v>1669</v>
+      </c>
       <c r="G92" s="1" t="s">
         <v>46</v>
       </c>
@@ -15045,6 +15312,9 @@
       <c r="E93" s="1" t="s">
         <v>475</v>
       </c>
+      <c r="F93" s="1">
+        <v>1669</v>
+      </c>
       <c r="G93" s="1" t="s">
         <v>46</v>
       </c>
@@ -15134,6 +15404,9 @@
       <c r="E94" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="F94" s="1">
+        <v>1669</v>
+      </c>
       <c r="G94" s="1" t="s">
         <v>46</v>
       </c>
@@ -15223,6 +15496,9 @@
       <c r="E95" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="F95" s="1">
+        <v>1669</v>
+      </c>
       <c r="G95" s="1" t="s">
         <v>46</v>
       </c>
@@ -15312,6 +15588,9 @@
       <c r="E96" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="F96" s="1">
+        <v>1669</v>
+      </c>
       <c r="G96" s="1" t="s">
         <v>46</v>
       </c>
@@ -15401,6 +15680,9 @@
       <c r="E97" s="1" t="s">
         <v>496</v>
       </c>
+      <c r="F97" s="1">
+        <v>1669</v>
+      </c>
       <c r="G97" s="1" t="s">
         <v>46</v>
       </c>
@@ -15493,6 +15775,9 @@
       <c r="E98" s="1" t="s">
         <v>496</v>
       </c>
+      <c r="F98" s="1">
+        <v>1669</v>
+      </c>
       <c r="G98" s="1" t="s">
         <v>46</v>
       </c>
@@ -15582,6 +15867,9 @@
       <c r="E99" s="1" t="s">
         <v>508</v>
       </c>
+      <c r="F99" s="1">
+        <v>1669</v>
+      </c>
       <c r="G99" s="1" t="s">
         <v>46</v>
       </c>
@@ -15659,6 +15947,9 @@
       <c r="E100" s="1" t="s">
         <v>513</v>
       </c>
+      <c r="F100" s="1">
+        <v>1669</v>
+      </c>
       <c r="G100" s="1" t="s">
         <v>46</v>
       </c>
@@ -15745,6 +16036,9 @@
       <c r="E101" s="1" t="s">
         <v>513</v>
       </c>
+      <c r="F101" s="1">
+        <v>1669</v>
+      </c>
       <c r="G101" s="1" t="s">
         <v>46</v>
       </c>
@@ -15831,6 +16125,9 @@
       <c r="E102" s="1" t="s">
         <v>520</v>
       </c>
+      <c r="F102" s="1">
+        <v>1669</v>
+      </c>
       <c r="G102" s="1" t="s">
         <v>46</v>
       </c>
@@ -15923,6 +16220,9 @@
       <c r="E103" s="1" t="s">
         <v>526</v>
       </c>
+      <c r="F103" s="1">
+        <v>1669</v>
+      </c>
       <c r="G103" s="1" t="s">
         <v>46</v>
       </c>
@@ -16009,6 +16309,9 @@
       <c r="E104" s="1" t="s">
         <v>531</v>
       </c>
+      <c r="F104" s="1">
+        <v>1669</v>
+      </c>
       <c r="G104" s="1" t="s">
         <v>46</v>
       </c>
@@ -16098,6 +16401,9 @@
       <c r="E105" s="1" t="s">
         <v>531</v>
       </c>
+      <c r="F105" s="1">
+        <v>1669</v>
+      </c>
       <c r="G105" s="1" t="s">
         <v>46</v>
       </c>
@@ -16184,6 +16490,9 @@
       <c r="E106" s="1" t="s">
         <v>542</v>
       </c>
+      <c r="F106" s="1">
+        <v>1669</v>
+      </c>
       <c r="G106" s="1" t="s">
         <v>46</v>
       </c>
@@ -16270,6 +16579,9 @@
       <c r="E107" s="1" t="s">
         <v>542</v>
       </c>
+      <c r="F107" s="1">
+        <v>1669</v>
+      </c>
       <c r="G107" s="1" t="s">
         <v>46</v>
       </c>
@@ -16356,6 +16668,9 @@
       <c r="E108" s="1" t="s">
         <v>542</v>
       </c>
+      <c r="F108" s="1">
+        <v>1669</v>
+      </c>
       <c r="G108" s="1" t="s">
         <v>46</v>
       </c>
@@ -16433,6 +16748,9 @@
       <c r="E109" s="1" t="s">
         <v>542</v>
       </c>
+      <c r="F109" s="1">
+        <v>1669</v>
+      </c>
       <c r="G109" s="1" t="s">
         <v>46</v>
       </c>
@@ -16519,6 +16837,9 @@
       <c r="E110" s="1" t="s">
         <v>542</v>
       </c>
+      <c r="F110" s="1">
+        <v>1669</v>
+      </c>
       <c r="G110" s="1" t="s">
         <v>46</v>
       </c>
@@ -16605,6 +16926,9 @@
       <c r="E111" s="1" t="s">
         <v>559</v>
       </c>
+      <c r="F111" s="1">
+        <v>1669</v>
+      </c>
       <c r="G111" s="1" t="s">
         <v>46</v>
       </c>
@@ -16682,6 +17006,9 @@
       <c r="E112" s="1" t="s">
         <v>559</v>
       </c>
+      <c r="F112" s="1">
+        <v>1669</v>
+      </c>
       <c r="G112" s="1" t="s">
         <v>46</v>
       </c>
@@ -16768,6 +17095,9 @@
       <c r="E113" s="1" t="s">
         <v>567</v>
       </c>
+      <c r="F113" s="1">
+        <v>1669</v>
+      </c>
       <c r="G113" s="1" t="s">
         <v>46</v>
       </c>
@@ -16854,6 +17184,9 @@
       <c r="E114" s="1" t="s">
         <v>567</v>
       </c>
+      <c r="F114" s="1">
+        <v>1669</v>
+      </c>
       <c r="G114" s="1" t="s">
         <v>46</v>
       </c>
@@ -16940,6 +17273,9 @@
       <c r="E115" s="1" t="s">
         <v>576</v>
       </c>
+      <c r="F115" s="1">
+        <v>1669</v>
+      </c>
       <c r="G115" s="1" t="s">
         <v>46</v>
       </c>
@@ -17032,6 +17368,9 @@
       <c r="E116" s="1" t="s">
         <v>587</v>
       </c>
+      <c r="F116" s="1">
+        <v>1669</v>
+      </c>
       <c r="G116" s="1" t="s">
         <v>46</v>
       </c>
@@ -17118,6 +17457,9 @@
       <c r="E117" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="F117" s="1">
+        <v>1669</v>
+      </c>
       <c r="G117" s="1" t="s">
         <v>85</v>
       </c>
@@ -17210,6 +17552,9 @@
       <c r="E118" s="1" t="s">
         <v>587</v>
       </c>
+      <c r="F118" s="1">
+        <v>1669</v>
+      </c>
       <c r="G118" s="1" t="s">
         <v>46</v>
       </c>
@@ -17296,6 +17641,9 @@
       <c r="E119" s="1" t="s">
         <v>587</v>
       </c>
+      <c r="F119" s="1">
+        <v>1669</v>
+      </c>
       <c r="G119" s="1" t="s">
         <v>46</v>
       </c>
@@ -17373,6 +17721,9 @@
       <c r="E120" s="1" t="s">
         <v>587</v>
       </c>
+      <c r="F120" s="1">
+        <v>1669</v>
+      </c>
       <c r="G120" s="1" t="s">
         <v>46</v>
       </c>
@@ -17459,6 +17810,9 @@
       <c r="E121" s="1" t="s">
         <v>587</v>
       </c>
+      <c r="F121" s="1">
+        <v>1669</v>
+      </c>
       <c r="G121" s="1" t="s">
         <v>46</v>
       </c>
@@ -17545,6 +17899,9 @@
       <c r="E122" s="1" t="s">
         <v>604</v>
       </c>
+      <c r="F122" s="1">
+        <v>1670</v>
+      </c>
       <c r="G122" s="1" t="s">
         <v>46</v>
       </c>
@@ -17631,6 +17988,9 @@
       <c r="E123" s="1" t="s">
         <v>609</v>
       </c>
+      <c r="F123" s="1">
+        <v>1670</v>
+      </c>
       <c r="G123" s="1" t="s">
         <v>85</v>
       </c>
@@ -17720,6 +18080,9 @@
       <c r="E124" s="1" t="s">
         <v>609</v>
       </c>
+      <c r="F124" s="1">
+        <v>1670</v>
+      </c>
       <c r="G124" s="1" t="s">
         <v>85</v>
       </c>
@@ -17809,6 +18172,9 @@
       <c r="E125" s="1" t="s">
         <v>620</v>
       </c>
+      <c r="F125" s="1">
+        <v>1670</v>
+      </c>
       <c r="G125" s="1" t="s">
         <v>46</v>
       </c>
@@ -17898,6 +18264,9 @@
       <c r="E126" s="1" t="s">
         <v>620</v>
       </c>
+      <c r="F126" s="1">
+        <v>1670</v>
+      </c>
       <c r="G126" s="1" t="s">
         <v>46</v>
       </c>
@@ -17987,6 +18356,9 @@
       <c r="E127" s="1" t="s">
         <v>620</v>
       </c>
+      <c r="F127" s="1">
+        <v>1670</v>
+      </c>
       <c r="G127" s="1" t="s">
         <v>46</v>
       </c>
@@ -18076,6 +18448,9 @@
       <c r="E128" s="1" t="s">
         <v>620</v>
       </c>
+      <c r="F128" s="1">
+        <v>1670</v>
+      </c>
       <c r="G128" s="1" t="s">
         <v>46</v>
       </c>
@@ -18165,6 +18540,9 @@
       <c r="E129" s="1" t="s">
         <v>639</v>
       </c>
+      <c r="F129" s="1">
+        <v>1671</v>
+      </c>
       <c r="G129" s="1" t="s">
         <v>46</v>
       </c>
@@ -18251,6 +18629,9 @@
       <c r="E130" s="1" t="s">
         <v>646</v>
       </c>
+      <c r="F130" s="1">
+        <v>1671</v>
+      </c>
       <c r="G130" s="1" t="s">
         <v>46</v>
       </c>
@@ -18340,6 +18721,9 @@
       <c r="E131" s="1" t="s">
         <v>646</v>
       </c>
+      <c r="F131" s="1">
+        <v>1671</v>
+      </c>
       <c r="G131" s="1" t="s">
         <v>46</v>
       </c>
@@ -18426,6 +18810,9 @@
       <c r="E132" s="1" t="s">
         <v>654</v>
       </c>
+      <c r="F132" s="1">
+        <v>1671</v>
+      </c>
       <c r="G132" s="1" t="s">
         <v>46</v>
       </c>
@@ -18509,6 +18896,9 @@
       <c r="E133" s="1" t="s">
         <v>658</v>
       </c>
+      <c r="F133" s="1">
+        <v>1671</v>
+      </c>
       <c r="G133" s="1" t="s">
         <v>46</v>
       </c>
@@ -18598,6 +18988,9 @@
       <c r="E134" s="1" t="s">
         <v>658</v>
       </c>
+      <c r="F134" s="1">
+        <v>1671</v>
+      </c>
       <c r="G134" s="1" t="s">
         <v>46</v>
       </c>
@@ -18684,6 +19077,9 @@
       <c r="E135" s="1" t="s">
         <v>666</v>
       </c>
+      <c r="F135" s="1">
+        <v>1671</v>
+      </c>
       <c r="G135" s="1" t="s">
         <v>46</v>
       </c>
@@ -18761,6 +19157,9 @@
       <c r="E136" s="1" t="s">
         <v>666</v>
       </c>
+      <c r="F136" s="1">
+        <v>1671</v>
+      </c>
       <c r="G136" s="1" t="s">
         <v>46</v>
       </c>
@@ -18838,6 +19237,9 @@
       <c r="E137" s="1" t="s">
         <v>658</v>
       </c>
+      <c r="F137" s="1">
+        <v>1671</v>
+      </c>
       <c r="G137" s="1" t="s">
         <v>46</v>
       </c>
@@ -18921,6 +19323,9 @@
       <c r="E138" s="1" t="s">
         <v>681</v>
       </c>
+      <c r="F138" s="1">
+        <v>1671</v>
+      </c>
       <c r="G138" s="1" t="s">
         <v>682</v>
       </c>
@@ -19010,6 +19415,9 @@
       <c r="E139" s="1" t="s">
         <v>690</v>
       </c>
+      <c r="F139" s="1">
+        <v>1671</v>
+      </c>
       <c r="G139" s="1" t="s">
         <v>46</v>
       </c>
@@ -19096,6 +19504,9 @@
       <c r="E140" s="1" t="s">
         <v>690</v>
       </c>
+      <c r="F140" s="1">
+        <v>1671</v>
+      </c>
       <c r="G140" s="1" t="s">
         <v>46</v>
       </c>
@@ -19182,6 +19593,9 @@
       <c r="E141" s="1" t="s">
         <v>700</v>
       </c>
+      <c r="F141" s="1">
+        <v>1671</v>
+      </c>
       <c r="G141" s="1" t="s">
         <v>46</v>
       </c>
@@ -19268,6 +19682,9 @@
       <c r="E142" s="1" t="s">
         <v>700</v>
       </c>
+      <c r="F142" s="1">
+        <v>1671</v>
+      </c>
       <c r="G142" s="1" t="s">
         <v>46</v>
       </c>
@@ -19342,6 +19759,9 @@
       <c r="E143" s="1" t="s">
         <v>709</v>
       </c>
+      <c r="F143" s="1">
+        <v>1671</v>
+      </c>
       <c r="G143" s="1" t="s">
         <v>46</v>
       </c>
@@ -19428,6 +19848,9 @@
       <c r="E144" s="1" t="s">
         <v>715</v>
       </c>
+      <c r="F144" s="1">
+        <v>1671</v>
+      </c>
       <c r="G144" s="1" t="s">
         <v>46</v>
       </c>
@@ -19517,6 +19940,9 @@
       <c r="E145" s="1" t="s">
         <v>721</v>
       </c>
+      <c r="F145" s="1">
+        <v>1671</v>
+      </c>
       <c r="G145" s="1" t="s">
         <v>46</v>
       </c>
@@ -19603,6 +20029,9 @@
       <c r="E146" s="1" t="s">
         <v>727</v>
       </c>
+      <c r="F146" s="1">
+        <v>1671</v>
+      </c>
       <c r="G146" s="1" t="s">
         <v>46</v>
       </c>
@@ -19689,6 +20118,9 @@
       <c r="E147" s="1" t="s">
         <v>733</v>
       </c>
+      <c r="F147" s="1">
+        <v>1671</v>
+      </c>
       <c r="G147" s="1" t="s">
         <v>46</v>
       </c>
@@ -19775,6 +20207,9 @@
       <c r="E148" s="1" t="s">
         <v>740</v>
       </c>
+      <c r="F148" s="1">
+        <v>1671</v>
+      </c>
       <c r="G148" s="1" t="s">
         <v>46</v>
       </c>
@@ -19852,6 +20287,9 @@
       <c r="E149" s="1" t="s">
         <v>740</v>
       </c>
+      <c r="F149" s="1">
+        <v>1671</v>
+      </c>
       <c r="G149" s="1" t="s">
         <v>46</v>
       </c>
@@ -19938,6 +20376,9 @@
       <c r="E150" s="1" t="s">
         <v>748</v>
       </c>
+      <c r="F150" s="1">
+        <v>1671</v>
+      </c>
       <c r="G150" s="1" t="s">
         <v>46</v>
       </c>
@@ -20024,6 +20465,9 @@
       <c r="E151" s="1" t="s">
         <v>755</v>
       </c>
+      <c r="F151" s="1">
+        <v>1672</v>
+      </c>
       <c r="G151" s="1" t="s">
         <v>46</v>
       </c>
@@ -20110,6 +20554,9 @@
       <c r="E152" s="1" t="s">
         <v>759</v>
       </c>
+      <c r="F152" s="1">
+        <v>1672</v>
+      </c>
       <c r="G152" s="1" t="s">
         <v>46</v>
       </c>
@@ -20196,6 +20643,9 @@
       <c r="E153" s="1" t="s">
         <v>764</v>
       </c>
+      <c r="F153" s="1">
+        <v>1672</v>
+      </c>
       <c r="G153" s="1" t="s">
         <v>46</v>
       </c>
@@ -20282,6 +20732,9 @@
       <c r="E154" s="1" t="s">
         <v>764</v>
       </c>
+      <c r="F154" s="1">
+        <v>1672</v>
+      </c>
       <c r="G154" s="1" t="s">
         <v>46</v>
       </c>
@@ -20368,6 +20821,9 @@
       <c r="E155" s="1" t="s">
         <v>774</v>
       </c>
+      <c r="F155" s="1">
+        <v>1672</v>
+      </c>
       <c r="G155" s="1" t="s">
         <v>46</v>
       </c>
@@ -20445,6 +20901,9 @@
       <c r="E156" s="1" t="s">
         <v>774</v>
       </c>
+      <c r="F156" s="1">
+        <v>1672</v>
+      </c>
       <c r="G156" s="1" t="s">
         <v>46</v>
       </c>
@@ -20531,6 +20990,9 @@
       <c r="E157" s="1" t="s">
         <v>774</v>
       </c>
+      <c r="F157" s="1">
+        <v>1672</v>
+      </c>
       <c r="G157" s="1" t="s">
         <v>46</v>
       </c>
@@ -20608,6 +21070,9 @@
       <c r="E158" s="1" t="s">
         <v>774</v>
       </c>
+      <c r="F158" s="1">
+        <v>1672</v>
+      </c>
       <c r="G158" s="1" t="s">
         <v>46</v>
       </c>
@@ -20694,6 +21159,9 @@
       <c r="E159" s="1" t="s">
         <v>790</v>
       </c>
+      <c r="F159" s="1">
+        <v>1672</v>
+      </c>
       <c r="G159" s="1" t="s">
         <v>46</v>
       </c>
@@ -20771,6 +21239,9 @@
       <c r="E160" s="1" t="s">
         <v>790</v>
       </c>
+      <c r="F160" s="1">
+        <v>1672</v>
+      </c>
       <c r="G160" s="1" t="s">
         <v>46</v>
       </c>
@@ -20848,6 +21319,9 @@
       <c r="E161" s="1" t="s">
         <v>790</v>
       </c>
+      <c r="F161" s="1">
+        <v>1672</v>
+      </c>
       <c r="G161" s="1" t="s">
         <v>46</v>
       </c>
@@ -20925,6 +21399,9 @@
       <c r="E162" s="1" t="s">
         <v>790</v>
       </c>
+      <c r="F162" s="1">
+        <v>1672</v>
+      </c>
       <c r="G162" s="1" t="s">
         <v>46</v>
       </c>
@@ -21011,6 +21488,9 @@
       <c r="E163" s="1" t="s">
         <v>808</v>
       </c>
+      <c r="F163" s="1">
+        <v>1672</v>
+      </c>
       <c r="G163" s="1" t="s">
         <v>46</v>
       </c>
@@ -21088,6 +21568,9 @@
       <c r="E164" s="1" t="s">
         <v>808</v>
       </c>
+      <c r="F164" s="1">
+        <v>1672</v>
+      </c>
       <c r="G164" s="1" t="s">
         <v>46</v>
       </c>
@@ -21165,6 +21648,9 @@
       <c r="E165" s="1" t="s">
         <v>816</v>
       </c>
+      <c r="F165" s="1">
+        <v>1672</v>
+      </c>
       <c r="G165" s="1" t="s">
         <v>46</v>
       </c>
@@ -21251,6 +21737,9 @@
       <c r="E166" s="1" t="s">
         <v>821</v>
       </c>
+      <c r="F166" s="1">
+        <v>1672</v>
+      </c>
       <c r="G166" s="1" t="s">
         <v>46</v>
       </c>
@@ -21337,6 +21826,9 @@
       <c r="E167" s="1" t="s">
         <v>828</v>
       </c>
+      <c r="F167" s="1">
+        <v>1672</v>
+      </c>
       <c r="G167" s="1" t="s">
         <v>31</v>
       </c>
@@ -21414,6 +21906,9 @@
       <c r="E168" s="1" t="s">
         <v>828</v>
       </c>
+      <c r="F168" s="1">
+        <v>1672</v>
+      </c>
       <c r="G168" s="1" t="s">
         <v>31</v>
       </c>
@@ -21503,6 +21998,9 @@
       <c r="E169" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F169" s="1">
+        <v>1672</v>
+      </c>
       <c r="G169" s="1" t="s">
         <v>46</v>
       </c>
@@ -21589,6 +22087,9 @@
       <c r="E170" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F170" s="1">
+        <v>1672</v>
+      </c>
       <c r="G170" s="1" t="s">
         <v>46</v>
       </c>
@@ -21675,6 +22176,9 @@
       <c r="E171" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F171" s="1">
+        <v>1672</v>
+      </c>
       <c r="G171" s="1" t="s">
         <v>46</v>
       </c>
@@ -21761,6 +22265,9 @@
       <c r="E172" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F172" s="1">
+        <v>1672</v>
+      </c>
       <c r="G172" s="1" t="s">
         <v>46</v>
       </c>
@@ -21847,6 +22354,9 @@
       <c r="E173" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F173" s="1">
+        <v>1672</v>
+      </c>
       <c r="G173" s="1" t="s">
         <v>46</v>
       </c>
@@ -21924,6 +22434,9 @@
       <c r="E174" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F174" s="1">
+        <v>1672</v>
+      </c>
       <c r="G174" s="1" t="s">
         <v>46</v>
       </c>
@@ -22010,6 +22523,9 @@
       <c r="E175" s="1" t="s">
         <v>856</v>
       </c>
+      <c r="F175" s="1">
+        <v>1672</v>
+      </c>
       <c r="G175" s="1" t="s">
         <v>46</v>
       </c>
@@ -22096,6 +22612,9 @@
       <c r="E176" s="1" t="s">
         <v>861</v>
       </c>
+      <c r="F176" s="1">
+        <v>1672</v>
+      </c>
       <c r="G176" s="1" t="s">
         <v>46</v>
       </c>
@@ -22173,6 +22692,9 @@
       <c r="E177" s="1" t="s">
         <v>861</v>
       </c>
+      <c r="F177" s="1">
+        <v>1672</v>
+      </c>
       <c r="G177" s="1" t="s">
         <v>46</v>
       </c>
@@ -22259,6 +22781,9 @@
       <c r="E178" s="1" t="s">
         <v>861</v>
       </c>
+      <c r="F178" s="1">
+        <v>1672</v>
+      </c>
       <c r="G178" s="1" t="s">
         <v>46</v>
       </c>
@@ -22345,6 +22870,9 @@
       <c r="E179" s="1" t="s">
         <v>872</v>
       </c>
+      <c r="F179" s="1">
+        <v>1672</v>
+      </c>
       <c r="G179" s="1" t="s">
         <v>46</v>
       </c>
@@ -22422,6 +22950,9 @@
       <c r="E180" s="1" t="s">
         <v>872</v>
       </c>
+      <c r="F180" s="1">
+        <v>1672</v>
+      </c>
       <c r="G180" s="1" t="s">
         <v>46</v>
       </c>
@@ -22508,6 +23039,9 @@
       <c r="E181" s="1" t="s">
         <v>882</v>
       </c>
+      <c r="F181" s="1">
+        <v>1672</v>
+      </c>
       <c r="G181" s="1" t="s">
         <v>31</v>
       </c>
@@ -22585,6 +23119,9 @@
       <c r="E182" s="1" t="s">
         <v>887</v>
       </c>
+      <c r="F182" s="1">
+        <v>1673</v>
+      </c>
       <c r="G182" s="1" t="s">
         <v>46</v>
       </c>
@@ -22671,6 +23208,9 @@
       <c r="E183" s="1" t="s">
         <v>887</v>
       </c>
+      <c r="F183" s="1">
+        <v>1673</v>
+      </c>
       <c r="G183" s="1" t="s">
         <v>46</v>
       </c>
@@ -22754,6 +23294,9 @@
       <c r="E184" s="1" t="s">
         <v>887</v>
       </c>
+      <c r="F184" s="1">
+        <v>1673</v>
+      </c>
       <c r="G184" s="1" t="s">
         <v>46</v>
       </c>
@@ -22840,6 +23383,9 @@
       <c r="E185" s="1" t="s">
         <v>887</v>
       </c>
+      <c r="F185" s="1">
+        <v>1673</v>
+      </c>
       <c r="G185" s="1" t="s">
         <v>46</v>
       </c>
@@ -22929,6 +23475,9 @@
       <c r="E186" s="1" t="s">
         <v>887</v>
       </c>
+      <c r="F186" s="1">
+        <v>1673</v>
+      </c>
       <c r="G186" s="1" t="s">
         <v>46</v>
       </c>
@@ -23015,6 +23564,9 @@
       <c r="E187" s="1" t="s">
         <v>908</v>
       </c>
+      <c r="F187" s="1">
+        <v>1674</v>
+      </c>
       <c r="G187" s="1" t="s">
         <v>46</v>
       </c>
@@ -23095,6 +23647,9 @@
       <c r="E188" s="1" t="s">
         <v>908</v>
       </c>
+      <c r="F188" s="1">
+        <v>1674</v>
+      </c>
       <c r="G188" s="1" t="s">
         <v>46</v>
       </c>
@@ -23184,6 +23739,9 @@
       <c r="E189" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F189" s="1">
+        <v>1675</v>
+      </c>
       <c r="G189" s="1" t="s">
         <v>46</v>
       </c>
@@ -23273,6 +23831,9 @@
       <c r="E190" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F190" s="1">
+        <v>1675</v>
+      </c>
       <c r="G190" s="1" t="s">
         <v>46</v>
       </c>
@@ -23359,6 +23920,9 @@
       <c r="E191" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F191" s="1">
+        <v>1675</v>
+      </c>
       <c r="G191" s="1" t="s">
         <v>46</v>
       </c>
@@ -23445,6 +24009,9 @@
       <c r="E192" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F192" s="1">
+        <v>1675</v>
+      </c>
       <c r="G192" s="1" t="s">
         <v>46</v>
       </c>
@@ -23531,6 +24098,9 @@
       <c r="E193" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F193" s="1">
+        <v>1675</v>
+      </c>
       <c r="G193" s="1" t="s">
         <v>46</v>
       </c>
@@ -23617,6 +24187,9 @@
       <c r="E194" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F194" s="1">
+        <v>1675</v>
+      </c>
       <c r="G194" s="1" t="s">
         <v>46</v>
       </c>
@@ -23703,6 +24276,9 @@
       <c r="E195" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="F195" s="1">
+        <v>1675</v>
+      </c>
       <c r="G195" s="1" t="s">
         <v>46</v>
       </c>
@@ -23792,6 +24368,9 @@
       <c r="E196" s="1" t="s">
         <v>944</v>
       </c>
+      <c r="F196" s="1">
+        <v>1675</v>
+      </c>
       <c r="G196" s="1" t="s">
         <v>46</v>
       </c>
@@ -23881,6 +24460,9 @@
       <c r="E197" s="1" t="s">
         <v>952</v>
       </c>
+      <c r="F197" s="1">
+        <v>1675</v>
+      </c>
       <c r="G197" s="1" t="s">
         <v>46</v>
       </c>
@@ -23967,6 +24549,9 @@
       <c r="E198" s="1" t="s">
         <v>952</v>
       </c>
+      <c r="F198" s="1">
+        <v>1675</v>
+      </c>
       <c r="G198" s="1" t="s">
         <v>46</v>
       </c>
@@ -24044,6 +24629,9 @@
       <c r="E199" s="1" t="s">
         <v>952</v>
       </c>
+      <c r="F199" s="1">
+        <v>1675</v>
+      </c>
       <c r="G199" s="1" t="s">
         <v>46</v>
       </c>
@@ -24133,6 +24721,9 @@
       <c r="E200" s="1" t="s">
         <v>971</v>
       </c>
+      <c r="F200" s="1">
+        <v>1674</v>
+      </c>
       <c r="G200" s="1" t="s">
         <v>31</v>
       </c>
@@ -24219,6 +24810,9 @@
       <c r="E201" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="F201" s="1">
+        <v>1675</v>
+      </c>
       <c r="G201" s="1" t="s">
         <v>31</v>
       </c>
@@ -24305,6 +24899,9 @@
       <c r="E202" s="1" t="s">
         <v>978</v>
       </c>
+      <c r="F202" s="1">
+        <v>1675</v>
+      </c>
       <c r="G202" s="1" t="s">
         <v>46</v>
       </c>
@@ -24382,6 +24979,9 @@
       <c r="E203" s="1" t="s">
         <v>978</v>
       </c>
+      <c r="F203" s="1">
+        <v>1675</v>
+      </c>
       <c r="G203" s="1" t="s">
         <v>31</v>
       </c>
@@ -24468,6 +25068,9 @@
       <c r="E204" s="1" t="s">
         <v>1002</v>
       </c>
+      <c r="F204" s="1">
+        <v>1675</v>
+      </c>
       <c r="G204" s="1" t="s">
         <v>31</v>
       </c>
@@ -24557,6 +25160,9 @@
       <c r="E205" s="1" t="s">
         <v>992</v>
       </c>
+      <c r="F205" s="1">
+        <v>1675</v>
+      </c>
       <c r="G205" s="1" t="s">
         <v>46</v>
       </c>
@@ -24643,6 +25249,9 @@
       <c r="E206" s="1" t="s">
         <v>992</v>
       </c>
+      <c r="F206" s="1">
+        <v>1675</v>
+      </c>
       <c r="G206" s="1" t="s">
         <v>46</v>
       </c>
@@ -24720,6 +25329,9 @@
       <c r="E207" s="1" t="s">
         <v>1008</v>
       </c>
+      <c r="F207" s="1">
+        <v>1675</v>
+      </c>
       <c r="G207" s="1" t="s">
         <v>46</v>
       </c>
@@ -24806,6 +25418,9 @@
       <c r="E208" s="1" t="s">
         <v>1008</v>
       </c>
+      <c r="F208" s="1">
+        <v>1675</v>
+      </c>
       <c r="G208" s="1" t="s">
         <v>46</v>
       </c>
@@ -24892,6 +25507,9 @@
       <c r="E209" s="1" t="s">
         <v>1016</v>
       </c>
+      <c r="F209" s="1">
+        <v>1675</v>
+      </c>
       <c r="G209" s="1" t="s">
         <v>31</v>
       </c>
@@ -24978,6 +25596,9 @@
       <c r="E210" s="1" t="s">
         <v>1021</v>
       </c>
+      <c r="F210" s="1">
+        <v>1675</v>
+      </c>
       <c r="G210" s="1" t="s">
         <v>46</v>
       </c>
@@ -25067,6 +25688,9 @@
       <c r="E211" s="1" t="s">
         <v>1027</v>
       </c>
+      <c r="F211" s="1">
+        <v>1675</v>
+      </c>
       <c r="G211" s="1" t="s">
         <v>31</v>
       </c>
@@ -25144,6 +25768,9 @@
       <c r="E212" s="1" t="s">
         <v>1034</v>
       </c>
+      <c r="F212" s="1">
+        <v>1675</v>
+      </c>
       <c r="G212" s="1" t="s">
         <v>31</v>
       </c>
@@ -25230,6 +25857,9 @@
       <c r="E213" s="1" t="s">
         <v>1041</v>
       </c>
+      <c r="F213" s="1">
+        <v>1675</v>
+      </c>
       <c r="G213" s="1" t="s">
         <v>46</v>
       </c>
@@ -25316,6 +25946,9 @@
       <c r="E214" s="1" t="s">
         <v>1041</v>
       </c>
+      <c r="F214" s="1">
+        <v>1675</v>
+      </c>
       <c r="G214" s="1" t="s">
         <v>46</v>
       </c>
@@ -25402,6 +26035,9 @@
       <c r="E215" s="1" t="s">
         <v>1041</v>
       </c>
+      <c r="F215" s="1">
+        <v>1675</v>
+      </c>
       <c r="G215" s="1" t="s">
         <v>46</v>
       </c>
@@ -25488,6 +26124,9 @@
       <c r="E216" s="1" t="s">
         <v>1041</v>
       </c>
+      <c r="F216" s="1">
+        <v>1675</v>
+      </c>
       <c r="G216" s="1" t="s">
         <v>46</v>
       </c>
@@ -25562,6 +26201,9 @@
       <c r="E217" s="1" t="s">
         <v>1056</v>
       </c>
+      <c r="F217" s="1">
+        <v>1675</v>
+      </c>
       <c r="G217" s="1" t="s">
         <v>85</v>
       </c>
@@ -25651,6 +26293,9 @@
       <c r="E218" s="1" t="s">
         <v>1064</v>
       </c>
+      <c r="F218" s="1">
+        <v>1675</v>
+      </c>
       <c r="G218" s="1" t="s">
         <v>31</v>
       </c>
@@ -25737,6 +26382,9 @@
       <c r="E219" s="1" t="s">
         <v>1074</v>
       </c>
+      <c r="F219" s="1">
+        <v>1675</v>
+      </c>
       <c r="G219" s="1" t="s">
         <v>85</v>
       </c>
@@ -25823,6 +26471,9 @@
       <c r="E220" s="1" t="s">
         <v>1069</v>
       </c>
+      <c r="F220" s="1">
+        <v>1675</v>
+      </c>
       <c r="G220" s="1" t="s">
         <v>31</v>
       </c>
@@ -25909,6 +26560,9 @@
       <c r="E221" s="1" t="s">
         <v>1082</v>
       </c>
+      <c r="F221" s="1">
+        <v>1675</v>
+      </c>
       <c r="G221" s="1" t="s">
         <v>46</v>
       </c>
@@ -25998,6 +26652,9 @@
       <c r="E222" s="1" t="s">
         <v>1089</v>
       </c>
+      <c r="F222" s="1">
+        <v>1675</v>
+      </c>
       <c r="G222" s="1" t="s">
         <v>46</v>
       </c>
@@ -26087,6 +26744,9 @@
       <c r="E223" s="1" t="s">
         <v>1089</v>
       </c>
+      <c r="F223" s="1">
+        <v>1675</v>
+      </c>
       <c r="G223" s="1" t="s">
         <v>46</v>
       </c>
@@ -26176,6 +26836,9 @@
       <c r="E224" s="1" t="s">
         <v>1089</v>
       </c>
+      <c r="F224" s="1">
+        <v>1675</v>
+      </c>
       <c r="G224" s="1" t="s">
         <v>46</v>
       </c>
@@ -26265,6 +26928,9 @@
       <c r="E225" s="1" t="s">
         <v>1089</v>
       </c>
+      <c r="F225" s="1">
+        <v>1675</v>
+      </c>
       <c r="G225" s="1" t="s">
         <v>46</v>
       </c>
@@ -26354,6 +27020,9 @@
       <c r="E226" s="1" t="s">
         <v>1104</v>
       </c>
+      <c r="F226" s="1">
+        <v>1675</v>
+      </c>
       <c r="G226" s="1" t="s">
         <v>46</v>
       </c>
@@ -26440,6 +27109,9 @@
       <c r="E227" s="1" t="s">
         <v>1110</v>
       </c>
+      <c r="F227" s="1">
+        <v>1675</v>
+      </c>
       <c r="G227" s="1" t="s">
         <v>46</v>
       </c>
@@ -26526,6 +27198,9 @@
       <c r="E228" s="1" t="s">
         <v>1115</v>
       </c>
+      <c r="F228" s="1">
+        <v>1676</v>
+      </c>
       <c r="G228" s="1" t="s">
         <v>31</v>
       </c>
@@ -26612,6 +27287,9 @@
       <c r="E229" s="1" t="s">
         <v>1115</v>
       </c>
+      <c r="F229" s="1">
+        <v>1676</v>
+      </c>
       <c r="G229" s="1" t="s">
         <v>31</v>
       </c>
@@ -26695,6 +27373,9 @@
       <c r="E230" s="1" t="s">
         <v>1115</v>
       </c>
+      <c r="F230" s="1">
+        <v>1676</v>
+      </c>
       <c r="G230" s="1" t="s">
         <v>31</v>
       </c>
@@ -26781,6 +27462,9 @@
       <c r="E231" s="1" t="s">
         <v>1128</v>
       </c>
+      <c r="F231" s="1">
+        <v>1676</v>
+      </c>
       <c r="G231" s="1" t="s">
         <v>85</v>
       </c>
@@ -26867,6 +27551,9 @@
       <c r="E232" s="1" t="s">
         <v>1137</v>
       </c>
+      <c r="F232" s="1">
+        <v>1675</v>
+      </c>
       <c r="G232" s="1" t="s">
         <v>46</v>
       </c>
@@ -26953,6 +27640,9 @@
       <c r="E233" s="1" t="s">
         <v>1142</v>
       </c>
+      <c r="F233" s="1">
+        <v>1676</v>
+      </c>
       <c r="G233" s="1" t="s">
         <v>31</v>
       </c>
@@ -27039,6 +27729,9 @@
       <c r="E234" s="1" t="s">
         <v>1148</v>
       </c>
+      <c r="F234" s="1">
+        <v>1676</v>
+      </c>
       <c r="G234" s="1" t="s">
         <v>46</v>
       </c>
@@ -27119,6 +27812,9 @@
       <c r="E235" s="1" t="s">
         <v>1148</v>
       </c>
+      <c r="F235" s="1">
+        <v>1676</v>
+      </c>
       <c r="G235" s="1" t="s">
         <v>46</v>
       </c>
@@ -27208,6 +27904,9 @@
       <c r="E236" s="1" t="s">
         <v>1148</v>
       </c>
+      <c r="F236" s="1">
+        <v>1676</v>
+      </c>
       <c r="G236" s="1" t="s">
         <v>46</v>
       </c>
@@ -27297,6 +27996,9 @@
       <c r="E237" s="1" t="s">
         <v>1161</v>
       </c>
+      <c r="F237" s="1">
+        <v>1676</v>
+      </c>
       <c r="G237" s="1" t="s">
         <v>1162</v>
       </c>
@@ -27371,6 +28073,9 @@
       <c r="E238" s="1" t="s">
         <v>1167</v>
       </c>
+      <c r="F238" s="1">
+        <v>1676</v>
+      </c>
       <c r="G238" s="1" t="s">
         <v>682</v>
       </c>
@@ -27457,6 +28162,9 @@
       <c r="E239" s="1" t="s">
         <v>1173</v>
       </c>
+      <c r="F239" s="1">
+        <v>1676</v>
+      </c>
       <c r="G239" s="1" t="s">
         <v>46</v>
       </c>
@@ -27546,6 +28254,9 @@
       <c r="E240" s="1" t="s">
         <v>1180</v>
       </c>
+      <c r="F240" s="1">
+        <v>1676</v>
+      </c>
       <c r="G240" s="1" t="s">
         <v>46</v>
       </c>
@@ -27623,6 +28334,9 @@
       <c r="E241" s="1" t="s">
         <v>1187</v>
       </c>
+      <c r="F241" s="1">
+        <v>1676</v>
+      </c>
       <c r="G241" s="1" t="s">
         <v>46</v>
       </c>
@@ -27709,6 +28423,9 @@
       <c r="E242" s="1" t="s">
         <v>1187</v>
       </c>
+      <c r="F242" s="1">
+        <v>1676</v>
+      </c>
       <c r="G242" s="1" t="s">
         <v>46</v>
       </c>
@@ -27786,6 +28503,9 @@
       <c r="E243" s="1" t="s">
         <v>1187</v>
       </c>
+      <c r="F243" s="1">
+        <v>1676</v>
+      </c>
       <c r="G243" s="1" t="s">
         <v>46</v>
       </c>
@@ -27872,6 +28592,9 @@
       <c r="E244" s="1" t="s">
         <v>1187</v>
       </c>
+      <c r="F244" s="1">
+        <v>1676</v>
+      </c>
       <c r="G244" s="1" t="s">
         <v>46</v>
       </c>
@@ -27949,6 +28672,9 @@
       <c r="E245" s="1" t="s">
         <v>1187</v>
       </c>
+      <c r="F245" s="1">
+        <v>1676</v>
+      </c>
       <c r="G245" s="1" t="s">
         <v>46</v>
       </c>
@@ -28026,6 +28752,9 @@
       <c r="E246" s="1" t="s">
         <v>1206</v>
       </c>
+      <c r="F246" s="1">
+        <v>1676</v>
+      </c>
       <c r="G246" s="1" t="s">
         <v>46</v>
       </c>
@@ -28112,6 +28841,9 @@
       <c r="E247" s="1" t="s">
         <v>1206</v>
       </c>
+      <c r="F247" s="1">
+        <v>1676</v>
+      </c>
       <c r="G247" s="1" t="s">
         <v>46</v>
       </c>
@@ -28189,6 +28921,9 @@
       <c r="E248" s="1" t="s">
         <v>1206</v>
       </c>
+      <c r="F248" s="1">
+        <v>1676</v>
+      </c>
       <c r="G248" s="1" t="s">
         <v>46</v>
       </c>
@@ -28266,6 +29001,9 @@
       <c r="E249" s="1" t="s">
         <v>1206</v>
       </c>
+      <c r="F249" s="1">
+        <v>1676</v>
+      </c>
       <c r="G249" s="1" t="s">
         <v>46</v>
       </c>
@@ -28352,6 +29090,9 @@
       <c r="E250" s="1" t="s">
         <v>1206</v>
       </c>
+      <c r="F250" s="1">
+        <v>1676</v>
+      </c>
       <c r="G250" s="1" t="s">
         <v>46</v>
       </c>
@@ -28438,6 +29179,9 @@
       <c r="E251" s="1" t="s">
         <v>1206</v>
       </c>
+      <c r="F251" s="1">
+        <v>1676</v>
+      </c>
       <c r="G251" s="1" t="s">
         <v>46</v>
       </c>
@@ -28512,6 +29256,9 @@
       <c r="E252" s="1" t="s">
         <v>1167</v>
       </c>
+      <c r="F252" s="1">
+        <v>1676</v>
+      </c>
       <c r="G252" s="1" t="s">
         <v>46</v>
       </c>
@@ -28592,6 +29339,9 @@
       <c r="E253" s="1" t="s">
         <v>1227</v>
       </c>
+      <c r="F253" s="1">
+        <v>1676</v>
+      </c>
       <c r="G253" s="1" t="s">
         <v>46</v>
       </c>
@@ -28678,6 +29428,9 @@
       <c r="E254" s="1" t="s">
         <v>1244</v>
       </c>
+      <c r="F254" s="1">
+        <v>1676</v>
+      </c>
       <c r="G254" s="1" t="s">
         <v>46</v>
       </c>
@@ -28764,6 +29517,9 @@
       <c r="E255" s="1" t="s">
         <v>1237</v>
       </c>
+      <c r="F255" s="1">
+        <v>1676</v>
+      </c>
       <c r="G255" s="1" t="s">
         <v>46</v>
       </c>
@@ -28850,6 +29606,9 @@
       <c r="E256" s="1" t="s">
         <v>1250</v>
       </c>
+      <c r="F256" s="1">
+        <v>1676</v>
+      </c>
       <c r="G256" s="1" t="s">
         <v>31</v>
       </c>
@@ -28936,6 +29695,9 @@
       <c r="E257" s="1" t="s">
         <v>1256</v>
       </c>
+      <c r="F257" s="1">
+        <v>1676</v>
+      </c>
       <c r="G257" s="1" t="s">
         <v>46</v>
       </c>
@@ -29022,6 +29784,9 @@
       <c r="E258" s="1" t="s">
         <v>1256</v>
       </c>
+      <c r="F258" s="1">
+        <v>1676</v>
+      </c>
       <c r="G258" s="1" t="s">
         <v>46</v>
       </c>
@@ -29108,6 +29873,9 @@
       <c r="E259" s="1" t="s">
         <v>1256</v>
       </c>
+      <c r="F259" s="1">
+        <v>1676</v>
+      </c>
       <c r="G259" s="1" t="s">
         <v>46</v>
       </c>
@@ -29194,6 +29962,9 @@
       <c r="E260" s="1" t="s">
         <v>1267</v>
       </c>
+      <c r="F260" s="1">
+        <v>1676</v>
+      </c>
       <c r="G260" s="1" t="s">
         <v>46</v>
       </c>
@@ -29274,6 +30045,9 @@
       <c r="E261" s="1" t="s">
         <v>1272</v>
       </c>
+      <c r="F261" s="1">
+        <v>1676</v>
+      </c>
       <c r="G261" s="1" t="s">
         <v>46</v>
       </c>
@@ -29360,6 +30134,9 @@
       <c r="E262" s="1" t="s">
         <v>1279</v>
       </c>
+      <c r="F262" s="1">
+        <v>1676</v>
+      </c>
       <c r="G262" s="1" t="s">
         <v>31</v>
       </c>
@@ -29437,6 +30214,9 @@
       <c r="E263" s="1" t="s">
         <v>1285</v>
       </c>
+      <c r="F263" s="1">
+        <v>1676</v>
+      </c>
       <c r="G263" s="1" t="s">
         <v>31</v>
       </c>
@@ -29526,6 +30306,9 @@
       <c r="E264" s="1" t="s">
         <v>1290</v>
       </c>
+      <c r="F264" s="1">
+        <v>1676</v>
+      </c>
       <c r="G264" s="1" t="s">
         <v>46</v>
       </c>
@@ -29606,6 +30389,9 @@
       <c r="E265" s="1" t="s">
         <v>1297</v>
       </c>
+      <c r="F265" s="1">
+        <v>1676</v>
+      </c>
       <c r="G265" s="1" t="s">
         <v>31</v>
       </c>
@@ -29692,6 +30478,9 @@
       <c r="E266" s="1" t="s">
         <v>1297</v>
       </c>
+      <c r="F266" s="1">
+        <v>1676</v>
+      </c>
       <c r="G266" s="1" t="s">
         <v>31</v>
       </c>
@@ -29778,6 +30567,9 @@
       <c r="E267" s="1" t="s">
         <v>1307</v>
       </c>
+      <c r="F267" s="1">
+        <v>1676</v>
+      </c>
       <c r="G267" s="1" t="s">
         <v>85</v>
       </c>
@@ -29864,6 +30656,9 @@
       <c r="E268" s="1" t="s">
         <v>1314</v>
       </c>
+      <c r="F268" s="1">
+        <v>1676</v>
+      </c>
       <c r="G268" s="1" t="s">
         <v>85</v>
       </c>
@@ -29950,6 +30745,9 @@
       <c r="E269" s="1" t="s">
         <v>1314</v>
       </c>
+      <c r="F269" s="1">
+        <v>1676</v>
+      </c>
       <c r="G269" s="1" t="s">
         <v>85</v>
       </c>
@@ -30039,6 +30837,9 @@
       <c r="E270" s="1" t="s">
         <v>1314</v>
       </c>
+      <c r="F270" s="1">
+        <v>1676</v>
+      </c>
       <c r="G270" s="1" t="s">
         <v>85</v>
       </c>
@@ -30125,6 +30926,9 @@
       <c r="E271" s="1" t="s">
         <v>1328</v>
       </c>
+      <c r="F271" s="1">
+        <v>1676</v>
+      </c>
       <c r="G271" s="1" t="s">
         <v>31</v>
       </c>
@@ -30211,6 +31015,9 @@
       <c r="E272" s="1" t="s">
         <v>1333</v>
       </c>
+      <c r="F272" s="1">
+        <v>1676</v>
+      </c>
       <c r="G272" s="1" t="s">
         <v>46</v>
       </c>
@@ -30297,6 +31104,9 @@
       <c r="E273" s="1" t="s">
         <v>1333</v>
       </c>
+      <c r="F273" s="1">
+        <v>1676</v>
+      </c>
       <c r="G273" s="1" t="s">
         <v>46</v>
       </c>
@@ -30383,6 +31193,9 @@
       <c r="E274" s="1" t="s">
         <v>1343</v>
       </c>
+      <c r="F274" s="1">
+        <v>1676</v>
+      </c>
       <c r="G274" s="1" t="s">
         <v>46</v>
       </c>
@@ -30463,6 +31276,9 @@
       <c r="E275" s="1" t="s">
         <v>1343</v>
       </c>
+      <c r="F275" s="1">
+        <v>1676</v>
+      </c>
       <c r="G275" s="1" t="s">
         <v>46</v>
       </c>
@@ -30552,6 +31368,9 @@
       <c r="E276" s="1" t="s">
         <v>1343</v>
       </c>
+      <c r="F276" s="1">
+        <v>1676</v>
+      </c>
       <c r="G276" s="1" t="s">
         <v>46</v>
       </c>
@@ -30641,6 +31460,9 @@
       <c r="E277" s="1" t="s">
         <v>1354</v>
       </c>
+      <c r="F277" s="1">
+        <v>1676</v>
+      </c>
       <c r="G277" s="1" t="s">
         <v>31</v>
       </c>
@@ -30727,6 +31549,9 @@
       <c r="E278" s="1" t="s">
         <v>1359</v>
       </c>
+      <c r="F278" s="1">
+        <v>1677</v>
+      </c>
       <c r="G278" s="1" t="s">
         <v>46</v>
       </c>
@@ -30813,6 +31638,9 @@
       <c r="E279" s="1" t="s">
         <v>1359</v>
       </c>
+      <c r="F279" s="1">
+        <v>1677</v>
+      </c>
       <c r="G279" s="1" t="s">
         <v>46</v>
       </c>
@@ -30899,6 +31727,9 @@
       <c r="E280" s="1" t="s">
         <v>1369</v>
       </c>
+      <c r="F280" s="1">
+        <v>1677</v>
+      </c>
       <c r="G280" s="1" t="s">
         <v>31</v>
       </c>
@@ -30988,6 +31819,9 @@
       <c r="E281" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="F281" s="1">
+        <v>1677</v>
+      </c>
       <c r="G281" s="1" t="s">
         <v>31</v>
       </c>
@@ -31074,6 +31908,9 @@
       <c r="E282" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="F282" s="1">
+        <v>1677</v>
+      </c>
       <c r="G282" s="1" t="s">
         <v>31</v>
       </c>
@@ -31160,6 +31997,9 @@
       <c r="E283" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="F283" s="1">
+        <v>1677</v>
+      </c>
       <c r="G283" s="1" t="s">
         <v>31</v>
       </c>
@@ -31246,6 +32086,9 @@
       <c r="E284" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="F284" s="1">
+        <v>1677</v>
+      </c>
       <c r="G284" s="1" t="s">
         <v>31</v>
       </c>
@@ -31332,6 +32175,9 @@
       <c r="E285" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="F285" s="1">
+        <v>1677</v>
+      </c>
       <c r="G285" s="1" t="s">
         <v>31</v>
       </c>
@@ -31418,6 +32264,9 @@
       <c r="E286" s="1" t="s">
         <v>1395</v>
       </c>
+      <c r="F286" s="1">
+        <v>1676</v>
+      </c>
       <c r="G286" s="1" t="s">
         <v>31</v>
       </c>
@@ -31495,6 +32344,9 @@
       <c r="E287" s="1" t="s">
         <v>1402</v>
       </c>
+      <c r="F287" s="1">
+        <v>1677</v>
+      </c>
       <c r="G287" s="1" t="s">
         <v>1162</v>
       </c>
@@ -31581,6 +32433,9 @@
       <c r="E288" s="1" t="s">
         <v>1402</v>
       </c>
+      <c r="F288" s="1">
+        <v>1677</v>
+      </c>
       <c r="G288" s="1" t="s">
         <v>1162</v>
       </c>
@@ -31667,6 +32522,9 @@
       <c r="E289" s="1" t="s">
         <v>1402</v>
       </c>
+      <c r="F289" s="1">
+        <v>1677</v>
+      </c>
       <c r="G289" s="1" t="s">
         <v>1162</v>
       </c>
@@ -31753,6 +32611,9 @@
       <c r="E290" s="1" t="s">
         <v>1402</v>
       </c>
+      <c r="F290" s="1">
+        <v>1677</v>
+      </c>
       <c r="G290" s="1" t="s">
         <v>1162</v>
       </c>
@@ -31839,6 +32700,9 @@
       <c r="E291" s="1" t="s">
         <v>1418</v>
       </c>
+      <c r="F291" s="1">
+        <v>1677</v>
+      </c>
       <c r="G291" s="1" t="s">
         <v>46</v>
       </c>
@@ -31925,6 +32789,9 @@
       <c r="E292" s="1" t="s">
         <v>1424</v>
       </c>
+      <c r="F292" s="1">
+        <v>1677</v>
+      </c>
       <c r="G292" s="1" t="s">
         <v>46</v>
       </c>
@@ -32011,6 +32878,9 @@
       <c r="E293" s="1" t="s">
         <v>1431</v>
       </c>
+      <c r="F293" s="1">
+        <v>1677</v>
+      </c>
       <c r="G293" s="1" t="s">
         <v>46</v>
       </c>
@@ -32097,6 +32967,9 @@
       <c r="E294" s="1" t="s">
         <v>1431</v>
       </c>
+      <c r="F294" s="1">
+        <v>1677</v>
+      </c>
       <c r="G294" s="1" t="s">
         <v>46</v>
       </c>
@@ -32174,6 +33047,9 @@
       <c r="E295" s="1" t="s">
         <v>1439</v>
       </c>
+      <c r="F295" s="1">
+        <v>1677</v>
+      </c>
       <c r="G295" s="1" t="s">
         <v>46</v>
       </c>
@@ -32435,6 +33311,9 @@
       <c r="E298" s="1" t="s">
         <v>1454</v>
       </c>
+      <c r="F298" s="1">
+        <v>1677</v>
+      </c>
       <c r="G298" s="1" t="s">
         <v>46</v>
       </c>
@@ -32512,6 +33391,9 @@
       <c r="E299" s="1" t="s">
         <v>1454</v>
       </c>
+      <c r="F299" s="1">
+        <v>1677</v>
+      </c>
       <c r="G299" s="1" t="s">
         <v>46</v>
       </c>
@@ -32598,6 +33480,9 @@
       <c r="E300" s="1" t="s">
         <v>1462</v>
       </c>
+      <c r="F300" s="1">
+        <v>1677</v>
+      </c>
       <c r="G300" s="1" t="s">
         <v>31</v>
       </c>
@@ -32687,6 +33572,9 @@
       <c r="E301" s="1" t="s">
         <v>1467</v>
       </c>
+      <c r="F301" s="1">
+        <v>1677</v>
+      </c>
       <c r="G301" s="1" t="s">
         <v>31</v>
       </c>
@@ -32776,6 +33664,9 @@
       <c r="E302" s="1" t="s">
         <v>1472</v>
       </c>
+      <c r="F302" s="1">
+        <v>1677</v>
+      </c>
       <c r="G302" s="1" t="s">
         <v>46</v>
       </c>
@@ -32862,6 +33753,9 @@
       <c r="E303" s="1" t="s">
         <v>1486</v>
       </c>
+      <c r="F303" s="1">
+        <v>1677</v>
+      </c>
       <c r="G303" s="1" t="s">
         <v>1162</v>
       </c>
@@ -32954,6 +33848,9 @@
       <c r="E304" s="1" t="s">
         <v>1486</v>
       </c>
+      <c r="F304" s="1">
+        <v>1677</v>
+      </c>
       <c r="G304" s="1" t="s">
         <v>1162</v>
       </c>
@@ -33043,6 +33940,9 @@
       <c r="E305" s="1" t="s">
         <v>1479</v>
       </c>
+      <c r="F305" s="1">
+        <v>1677</v>
+      </c>
       <c r="G305" s="1" t="s">
         <v>46</v>
       </c>
@@ -33129,6 +34029,9 @@
       <c r="E306" s="1" t="s">
         <v>1494</v>
       </c>
+      <c r="F306" s="1">
+        <v>1677</v>
+      </c>
       <c r="G306" s="1" t="s">
         <v>85</v>
       </c>
@@ -33215,6 +34118,9 @@
       <c r="E307" s="1" t="s">
         <v>1502</v>
       </c>
+      <c r="F307" s="1">
+        <v>1677</v>
+      </c>
       <c r="G307" s="1" t="s">
         <v>31</v>
       </c>
@@ -33292,6 +34198,9 @@
       <c r="E308" s="1" t="s">
         <v>1502</v>
       </c>
+      <c r="F308" s="1">
+        <v>1677</v>
+      </c>
       <c r="G308" s="1" t="s">
         <v>31</v>
       </c>
@@ -33381,6 +34290,9 @@
       <c r="E309" s="1" t="s">
         <v>1512</v>
       </c>
+      <c r="F309" s="1">
+        <v>1677</v>
+      </c>
       <c r="G309" s="1" t="s">
         <v>46</v>
       </c>
@@ -33470,6 +34382,9 @@
       <c r="E310" s="1" t="s">
         <v>1512</v>
       </c>
+      <c r="F310" s="1">
+        <v>1677</v>
+      </c>
       <c r="G310" s="1" t="s">
         <v>46</v>
       </c>
@@ -33559,6 +34474,9 @@
       <c r="E311" s="1" t="s">
         <v>1512</v>
       </c>
+      <c r="F311" s="1">
+        <v>1677</v>
+      </c>
       <c r="G311" s="1" t="s">
         <v>46</v>
       </c>
@@ -33648,6 +34566,9 @@
       <c r="E312" s="1" t="s">
         <v>1523</v>
       </c>
+      <c r="F312" s="1">
+        <v>1677</v>
+      </c>
       <c r="G312" s="1" t="s">
         <v>46</v>
       </c>
@@ -33734,6 +34655,9 @@
       <c r="E313" s="1" t="s">
         <v>1530</v>
       </c>
+      <c r="F313" s="1">
+        <v>1677</v>
+      </c>
       <c r="G313" s="1" t="s">
         <v>1162</v>
       </c>
@@ -33820,6 +34744,9 @@
       <c r="E314" s="1" t="s">
         <v>1530</v>
       </c>
+      <c r="F314" s="1">
+        <v>1677</v>
+      </c>
       <c r="G314" s="1" t="s">
         <v>1162</v>
       </c>
@@ -33906,6 +34833,9 @@
       <c r="E315" s="1" t="s">
         <v>1537</v>
       </c>
+      <c r="F315" s="1">
+        <v>1677</v>
+      </c>
       <c r="G315" s="1" t="s">
         <v>46</v>
       </c>
@@ -33992,6 +34922,9 @@
       <c r="E316" s="1" t="s">
         <v>1542</v>
       </c>
+      <c r="F316" s="1">
+        <v>1678</v>
+      </c>
       <c r="G316" s="1" t="s">
         <v>46</v>
       </c>
@@ -34069,6 +35002,9 @@
       <c r="E317" s="1" t="s">
         <v>1542</v>
       </c>
+      <c r="F317" s="1">
+        <v>1678</v>
+      </c>
       <c r="G317" s="1" t="s">
         <v>46</v>
       </c>
@@ -34155,6 +35091,9 @@
       <c r="E318" s="1" t="s">
         <v>1542</v>
       </c>
+      <c r="F318" s="1">
+        <v>1678</v>
+      </c>
       <c r="G318" s="1" t="s">
         <v>46</v>
       </c>
@@ -34241,6 +35180,9 @@
       <c r="E319" s="1" t="s">
         <v>1553</v>
       </c>
+      <c r="F319" s="1">
+        <v>1678</v>
+      </c>
       <c r="G319" s="1" t="s">
         <v>31</v>
       </c>
@@ -34327,6 +35269,9 @@
       <c r="E320" s="1" t="s">
         <v>1558</v>
       </c>
+      <c r="F320" s="1">
+        <v>1678</v>
+      </c>
       <c r="G320" s="1" t="s">
         <v>46</v>
       </c>
@@ -34413,6 +35358,9 @@
       <c r="E321" s="1" t="s">
         <v>1558</v>
       </c>
+      <c r="F321" s="1">
+        <v>1678</v>
+      </c>
       <c r="G321" s="1" t="s">
         <v>46</v>
       </c>
@@ -34499,6 +35447,9 @@
       <c r="E322" s="1" t="s">
         <v>1558</v>
       </c>
+      <c r="F322" s="1">
+        <v>1678</v>
+      </c>
       <c r="G322" s="1" t="s">
         <v>46</v>
       </c>
@@ -34585,6 +35536,9 @@
       <c r="E323" s="1" t="s">
         <v>1558</v>
       </c>
+      <c r="F323" s="1">
+        <v>1678</v>
+      </c>
       <c r="G323" s="1" t="s">
         <v>46</v>
       </c>
@@ -34671,6 +35625,9 @@
       <c r="E324" s="1" t="s">
         <v>1573</v>
       </c>
+      <c r="F324" s="1">
+        <v>1678</v>
+      </c>
       <c r="G324" s="1" t="s">
         <v>31</v>
       </c>
@@ -34757,6 +35714,9 @@
       <c r="E325" s="1" t="s">
         <v>1573</v>
       </c>
+      <c r="F325" s="1">
+        <v>1678</v>
+      </c>
       <c r="G325" s="1" t="s">
         <v>31</v>
       </c>
@@ -34843,6 +35803,9 @@
       <c r="E326" s="1" t="s">
         <v>1583</v>
       </c>
+      <c r="F326" s="1">
+        <v>1678</v>
+      </c>
       <c r="G326" s="1" t="s">
         <v>1162</v>
       </c>
@@ -34920,6 +35883,9 @@
       <c r="E327" s="1" t="s">
         <v>1592</v>
       </c>
+      <c r="F327" s="1">
+        <v>1678</v>
+      </c>
       <c r="G327" s="1" t="s">
         <v>31</v>
       </c>
@@ -35006,6 +35972,9 @@
       <c r="E328" s="1" t="s">
         <v>1592</v>
       </c>
+      <c r="F328" s="1">
+        <v>1678</v>
+      </c>
       <c r="G328" s="1" t="s">
         <v>31</v>
       </c>
@@ -35092,6 +36061,9 @@
       <c r="E329" s="1" t="s">
         <v>1583</v>
       </c>
+      <c r="F329" s="1">
+        <v>1678</v>
+      </c>
       <c r="G329" s="1" t="s">
         <v>1162</v>
       </c>
@@ -35178,6 +36150,9 @@
       <c r="E330" s="1" t="s">
         <v>1602</v>
       </c>
+      <c r="F330" s="1">
+        <v>1678</v>
+      </c>
       <c r="G330" s="1" t="s">
         <v>31</v>
       </c>
@@ -35255,6 +36230,9 @@
       <c r="E331" s="1" t="s">
         <v>1602</v>
       </c>
+      <c r="F331" s="1">
+        <v>1678</v>
+      </c>
       <c r="G331" s="1" t="s">
         <v>31</v>
       </c>
@@ -35335,6 +36313,9 @@
       <c r="E332" s="1" t="s">
         <v>1610</v>
       </c>
+      <c r="F332" s="1">
+        <v>1678</v>
+      </c>
       <c r="G332" s="1" t="s">
         <v>1162</v>
       </c>
@@ -35412,6 +36393,9 @@
       <c r="E333" s="1" t="s">
         <v>1610</v>
       </c>
+      <c r="F333" s="1">
+        <v>1678</v>
+      </c>
       <c r="G333" s="1" t="s">
         <v>1162</v>
       </c>
@@ -35498,6 +36482,9 @@
       <c r="E334" s="1" t="s">
         <v>1618</v>
       </c>
+      <c r="F334" s="1">
+        <v>1678</v>
+      </c>
       <c r="G334" s="1" t="s">
         <v>46</v>
       </c>
@@ -35584,6 +36571,9 @@
       <c r="E335" s="1" t="s">
         <v>1623</v>
       </c>
+      <c r="F335" s="1">
+        <v>1678</v>
+      </c>
       <c r="G335" s="1" t="s">
         <v>46</v>
       </c>
@@ -35670,6 +36660,9 @@
       <c r="E336" s="1" t="s">
         <v>1623</v>
       </c>
+      <c r="F336" s="1">
+        <v>1678</v>
+      </c>
       <c r="G336" s="1" t="s">
         <v>46</v>
       </c>
@@ -35756,6 +36749,9 @@
       <c r="E337" s="1" t="s">
         <v>1634</v>
       </c>
+      <c r="F337" s="1">
+        <v>1678</v>
+      </c>
       <c r="G337" s="1" t="s">
         <v>31</v>
       </c>
@@ -35842,6 +36838,9 @@
       <c r="E338" s="1" t="s">
         <v>1639</v>
       </c>
+      <c r="F338" s="1">
+        <v>1678</v>
+      </c>
       <c r="G338" s="1" t="s">
         <v>31</v>
       </c>
@@ -35928,6 +36927,9 @@
       <c r="E339" s="1" t="s">
         <v>1644</v>
       </c>
+      <c r="F339" s="1">
+        <v>1678</v>
+      </c>
       <c r="G339" s="1" t="s">
         <v>85</v>
       </c>
@@ -36014,6 +37016,9 @@
       <c r="E340" s="1" t="s">
         <v>1651</v>
       </c>
+      <c r="F340" s="1">
+        <v>1678</v>
+      </c>
       <c r="G340" s="1" t="s">
         <v>31</v>
       </c>
@@ -36100,6 +37105,9 @@
       <c r="E341" s="1" t="s">
         <v>1651</v>
       </c>
+      <c r="F341" s="1">
+        <v>1678</v>
+      </c>
       <c r="G341" s="1" t="s">
         <v>46</v>
       </c>
@@ -36186,6 +37194,9 @@
       <c r="E342" s="1" t="s">
         <v>1660</v>
       </c>
+      <c r="F342" s="1">
+        <v>1678</v>
+      </c>
       <c r="G342" s="1" t="s">
         <v>46</v>
       </c>
@@ -36275,6 +37286,9 @@
       <c r="E343" s="1" t="s">
         <v>1665</v>
       </c>
+      <c r="F343" s="1">
+        <v>1678</v>
+      </c>
       <c r="G343" s="1" t="s">
         <v>46</v>
       </c>
@@ -36352,6 +37366,9 @@
       <c r="E344" s="1" t="s">
         <v>1672</v>
       </c>
+      <c r="F344" s="1">
+        <v>1678</v>
+      </c>
       <c r="G344" s="1" t="s">
         <v>31</v>
       </c>
@@ -36438,6 +37455,9 @@
       <c r="E345" s="1" t="s">
         <v>1677</v>
       </c>
+      <c r="F345" s="1">
+        <v>1678</v>
+      </c>
       <c r="G345" s="1" t="s">
         <v>46</v>
       </c>
@@ -36524,6 +37544,9 @@
       <c r="E346" s="1" t="s">
         <v>1677</v>
       </c>
+      <c r="F346" s="1">
+        <v>1678</v>
+      </c>
       <c r="G346" s="1" t="s">
         <v>46</v>
       </c>
@@ -36610,6 +37633,9 @@
       <c r="E347" s="1" t="s">
         <v>1685</v>
       </c>
+      <c r="F347" s="1">
+        <v>1678</v>
+      </c>
       <c r="G347" s="1" t="s">
         <v>85</v>
       </c>
@@ -36696,6 +37722,9 @@
       <c r="E348" s="1" t="s">
         <v>1692</v>
       </c>
+      <c r="F348" s="1">
+        <v>1678</v>
+      </c>
       <c r="G348" s="1" t="s">
         <v>85</v>
       </c>
@@ -36773,6 +37802,9 @@
       <c r="E349" s="1" t="s">
         <v>1698</v>
       </c>
+      <c r="F349" s="1">
+        <v>1678</v>
+      </c>
       <c r="G349" s="1" t="s">
         <v>31</v>
       </c>
@@ -36859,6 +37891,9 @@
       <c r="E350" s="1" t="s">
         <v>1703</v>
       </c>
+      <c r="F350" s="1">
+        <v>1678</v>
+      </c>
       <c r="G350" s="1" t="s">
         <v>1162</v>
       </c>
@@ -36945,6 +37980,9 @@
       <c r="E351" s="1" t="s">
         <v>1716</v>
       </c>
+      <c r="F351" s="1">
+        <v>1678</v>
+      </c>
       <c r="G351" s="1" t="s">
         <v>46</v>
       </c>
@@ -37031,6 +38069,9 @@
       <c r="E352" s="1" t="s">
         <v>1707</v>
       </c>
+      <c r="F352" s="1">
+        <v>1678</v>
+      </c>
       <c r="G352" s="1" t="s">
         <v>682</v>
       </c>
@@ -37111,6 +38152,9 @@
       <c r="E353" s="1" t="s">
         <v>1707</v>
       </c>
+      <c r="F353" s="1">
+        <v>1678</v>
+      </c>
       <c r="G353" s="1" t="s">
         <v>682</v>
       </c>
@@ -37191,6 +38235,9 @@
       <c r="E354" s="1" t="s">
         <v>1723</v>
       </c>
+      <c r="F354" s="1">
+        <v>1678</v>
+      </c>
       <c r="G354" s="1" t="s">
         <v>1162</v>
       </c>
@@ -37277,6 +38324,9 @@
       <c r="E355" s="1" t="s">
         <v>1727</v>
       </c>
+      <c r="F355" s="1">
+        <v>1679</v>
+      </c>
       <c r="G355" s="1" t="s">
         <v>46</v>
       </c>
@@ -37363,6 +38413,9 @@
       <c r="E356" s="1" t="s">
         <v>1727</v>
       </c>
+      <c r="F356" s="1">
+        <v>1679</v>
+      </c>
       <c r="G356" s="1" t="s">
         <v>46</v>
       </c>
@@ -37449,6 +38502,9 @@
       <c r="E357" s="1" t="s">
         <v>1735</v>
       </c>
+      <c r="F357" s="1">
+        <v>1679</v>
+      </c>
       <c r="G357" s="1" t="s">
         <v>85</v>
       </c>
@@ -37535,6 +38591,9 @@
       <c r="E358" s="1" t="s">
         <v>1735</v>
       </c>
+      <c r="F358" s="1">
+        <v>1679</v>
+      </c>
       <c r="G358" s="1" t="s">
         <v>85</v>
       </c>
@@ -37618,6 +38677,9 @@
       <c r="E359" s="1" t="s">
         <v>1735</v>
       </c>
+      <c r="F359" s="1">
+        <v>1679</v>
+      </c>
       <c r="G359" s="1" t="s">
         <v>85</v>
       </c>
@@ -37695,6 +38757,9 @@
       <c r="E360" s="1" t="s">
         <v>1735</v>
       </c>
+      <c r="F360" s="1">
+        <v>1679</v>
+      </c>
       <c r="G360" s="1" t="s">
         <v>85</v>
       </c>
@@ -37772,6 +38837,9 @@
       <c r="E361" s="1" t="s">
         <v>1752</v>
       </c>
+      <c r="F361" s="1">
+        <v>1678</v>
+      </c>
       <c r="G361" s="1" t="s">
         <v>31</v>
       </c>
@@ -37861,6 +38929,9 @@
       <c r="E362" s="1" t="s">
         <v>1757</v>
       </c>
+      <c r="F362" s="1">
+        <v>1679</v>
+      </c>
       <c r="G362" s="1" t="s">
         <v>46</v>
       </c>
@@ -37947,6 +39018,9 @@
       <c r="E363" s="1" t="s">
         <v>1763</v>
       </c>
+      <c r="F363" s="1">
+        <v>1679</v>
+      </c>
       <c r="G363" s="1" t="s">
         <v>46</v>
       </c>
@@ -38033,6 +39107,9 @@
       <c r="E364" s="1" t="s">
         <v>1763</v>
       </c>
+      <c r="F364" s="1">
+        <v>1679</v>
+      </c>
       <c r="G364" s="1" t="s">
         <v>46</v>
       </c>
@@ -38119,6 +39196,9 @@
       <c r="E365" s="1" t="s">
         <v>1772</v>
       </c>
+      <c r="F365" s="1">
+        <v>1679</v>
+      </c>
       <c r="G365" s="1" t="s">
         <v>46</v>
       </c>
@@ -38205,6 +39285,9 @@
       <c r="E366" s="1" t="s">
         <v>1772</v>
       </c>
+      <c r="F366" s="1">
+        <v>1679</v>
+      </c>
       <c r="G366" s="1" t="s">
         <v>46</v>
       </c>
@@ -38291,6 +39374,9 @@
       <c r="E367" s="1" t="s">
         <v>1782</v>
       </c>
+      <c r="F367" s="1">
+        <v>1679</v>
+      </c>
       <c r="G367" s="1" t="s">
         <v>46</v>
       </c>
@@ -38380,6 +39466,9 @@
       <c r="E368" s="1" t="s">
         <v>1788</v>
       </c>
+      <c r="F368" s="1">
+        <v>1679</v>
+      </c>
       <c r="G368" s="1" t="s">
         <v>85</v>
       </c>
@@ -38463,6 +39552,9 @@
       <c r="E369" s="1" t="s">
         <v>1788</v>
       </c>
+      <c r="F369" s="1">
+        <v>1679</v>
+      </c>
       <c r="G369" s="1" t="s">
         <v>85</v>
       </c>
@@ -38543,6 +39635,9 @@
       <c r="E370" s="1" t="s">
         <v>1788</v>
       </c>
+      <c r="F370" s="1">
+        <v>1679</v>
+      </c>
       <c r="G370" s="1" t="s">
         <v>85</v>
       </c>
@@ -38623,6 +39718,9 @@
       <c r="E371" s="1" t="s">
         <v>1788</v>
       </c>
+      <c r="F371" s="1">
+        <v>1679</v>
+      </c>
       <c r="G371" s="1" t="s">
         <v>85</v>
       </c>
@@ -38703,6 +39801,9 @@
       <c r="E372" s="1" t="s">
         <v>1788</v>
       </c>
+      <c r="F372" s="1">
+        <v>1679</v>
+      </c>
       <c r="G372" s="1" t="s">
         <v>85</v>
       </c>
@@ -38783,6 +39884,9 @@
       <c r="E373" s="1" t="s">
         <v>1788</v>
       </c>
+      <c r="F373" s="1">
+        <v>1679</v>
+      </c>
       <c r="G373" s="1" t="s">
         <v>85</v>
       </c>
@@ -38872,6 +39976,9 @@
       <c r="E374" s="1" t="s">
         <v>1812</v>
       </c>
+      <c r="F374" s="1">
+        <v>1679</v>
+      </c>
       <c r="G374" s="1" t="s">
         <v>46</v>
       </c>
@@ -38958,6 +40065,9 @@
       <c r="E375" s="1" t="s">
         <v>1817</v>
       </c>
+      <c r="F375" s="1">
+        <v>1679</v>
+      </c>
       <c r="G375" s="1" t="s">
         <v>1162</v>
       </c>
@@ -39044,6 +40154,9 @@
       <c r="E376" s="1" t="s">
         <v>1821</v>
       </c>
+      <c r="F376" s="1">
+        <v>1679</v>
+      </c>
       <c r="G376" s="1" t="s">
         <v>85</v>
       </c>
@@ -39133,6 +40246,9 @@
       <c r="E377" s="1" t="s">
         <v>1826</v>
       </c>
+      <c r="F377" s="1">
+        <v>1679</v>
+      </c>
       <c r="G377" s="1" t="s">
         <v>85</v>
       </c>
@@ -39222,6 +40338,9 @@
       <c r="E378" s="1" t="s">
         <v>1831</v>
       </c>
+      <c r="F378" s="1">
+        <v>1679</v>
+      </c>
       <c r="G378" s="1" t="s">
         <v>1162</v>
       </c>
@@ -39308,6 +40427,9 @@
       <c r="E379" s="1" t="s">
         <v>1831</v>
       </c>
+      <c r="F379" s="1">
+        <v>1679</v>
+      </c>
       <c r="G379" s="1" t="s">
         <v>1162</v>
       </c>
@@ -39394,6 +40516,9 @@
       <c r="E380" s="1" t="s">
         <v>1831</v>
       </c>
+      <c r="F380" s="1">
+        <v>1679</v>
+      </c>
       <c r="G380" s="1" t="s">
         <v>1162</v>
       </c>
@@ -39480,6 +40605,9 @@
       <c r="E381" s="1" t="s">
         <v>1844</v>
       </c>
+      <c r="F381" s="1">
+        <v>1679</v>
+      </c>
       <c r="G381" s="1" t="s">
         <v>46</v>
       </c>
@@ -39566,6 +40694,9 @@
       <c r="E382" s="1" t="s">
         <v>1856</v>
       </c>
+      <c r="F382" s="1">
+        <v>1679</v>
+      </c>
       <c r="G382" s="1" t="s">
         <v>31</v>
       </c>
@@ -39652,6 +40783,9 @@
       <c r="E383" s="1" t="s">
         <v>1844</v>
       </c>
+      <c r="F383" s="1">
+        <v>1679</v>
+      </c>
       <c r="G383" s="1" t="s">
         <v>46</v>
       </c>
@@ -39738,6 +40872,9 @@
       <c r="E384" s="1" t="s">
         <v>1844</v>
       </c>
+      <c r="F384" s="1">
+        <v>1679</v>
+      </c>
       <c r="G384" s="1" t="s">
         <v>46</v>
       </c>
@@ -39824,6 +40961,9 @@
       <c r="E385" s="1" t="s">
         <v>1861</v>
       </c>
+      <c r="F385" s="1">
+        <v>1679</v>
+      </c>
       <c r="G385" s="1" t="s">
         <v>46</v>
       </c>
@@ -39910,6 +41050,9 @@
       <c r="E386" s="1" t="s">
         <v>1866</v>
       </c>
+      <c r="F386" s="1">
+        <v>1679</v>
+      </c>
       <c r="G386" s="1" t="s">
         <v>46</v>
       </c>
@@ -39996,6 +41139,9 @@
       <c r="E387" s="1" t="s">
         <v>1870</v>
       </c>
+      <c r="F387" s="1">
+        <v>1679</v>
+      </c>
       <c r="G387" s="1" t="s">
         <v>31</v>
       </c>
@@ -40082,6 +41228,9 @@
       <c r="E388" s="1" t="s">
         <v>1875</v>
       </c>
+      <c r="F388" s="1">
+        <v>1679</v>
+      </c>
       <c r="G388" s="1" t="s">
         <v>31</v>
       </c>
@@ -40168,6 +41317,9 @@
       <c r="E389" s="1" t="s">
         <v>1875</v>
       </c>
+      <c r="F389" s="1">
+        <v>1679</v>
+      </c>
       <c r="G389" s="1" t="s">
         <v>31</v>
       </c>
@@ -40245,6 +41397,9 @@
       <c r="E390" s="1" t="s">
         <v>1885</v>
       </c>
+      <c r="F390" s="1">
+        <v>1679</v>
+      </c>
       <c r="G390" s="1" t="s">
         <v>31</v>
       </c>
@@ -40334,6 +41489,9 @@
       <c r="E391" s="1" t="s">
         <v>1891</v>
       </c>
+      <c r="F391" s="1">
+        <v>1679</v>
+      </c>
       <c r="G391" s="1" t="s">
         <v>1162</v>
       </c>
@@ -40423,6 +41581,9 @@
       <c r="E392" s="1" t="s">
         <v>1891</v>
       </c>
+      <c r="F392" s="1">
+        <v>1679</v>
+      </c>
       <c r="G392" s="1" t="s">
         <v>1162</v>
       </c>
@@ -40512,6 +41673,9 @@
       <c r="E393" s="1" t="s">
         <v>1891</v>
       </c>
+      <c r="F393" s="1">
+        <v>1679</v>
+      </c>
       <c r="G393" s="1" t="s">
         <v>1162</v>
       </c>
@@ -40589,6 +41753,9 @@
       <c r="E394" s="1" t="s">
         <v>1901</v>
       </c>
+      <c r="F394" s="1">
+        <v>1679</v>
+      </c>
       <c r="G394" s="1" t="s">
         <v>46</v>
       </c>
@@ -40675,6 +41842,9 @@
       <c r="E395" s="1" t="s">
         <v>1901</v>
       </c>
+      <c r="F395" s="1">
+        <v>1679</v>
+      </c>
       <c r="G395" s="1" t="s">
         <v>46</v>
       </c>
@@ -40761,6 +41931,9 @@
       <c r="E396" s="1" t="s">
         <v>1909</v>
       </c>
+      <c r="F396" s="1">
+        <v>1679</v>
+      </c>
       <c r="G396" s="1" t="s">
         <v>31</v>
       </c>
@@ -40847,6 +42020,9 @@
       <c r="E397" s="1" t="s">
         <v>1914</v>
       </c>
+      <c r="F397" s="1">
+        <v>1679</v>
+      </c>
       <c r="G397" s="1" t="s">
         <v>682</v>
       </c>
@@ -40927,6 +42103,9 @@
       <c r="E398" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F398" s="1">
+        <v>1679</v>
+      </c>
       <c r="G398" s="1" t="s">
         <v>46</v>
       </c>
@@ -41007,6 +42186,9 @@
       <c r="E399" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F399" s="1">
+        <v>1679</v>
+      </c>
       <c r="G399" s="1" t="s">
         <v>46</v>
       </c>
@@ -41087,6 +42269,9 @@
       <c r="E400" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F400" s="1">
+        <v>1679</v>
+      </c>
       <c r="G400" s="1" t="s">
         <v>46</v>
       </c>
@@ -41167,6 +42352,9 @@
       <c r="E401" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F401" s="1">
+        <v>1679</v>
+      </c>
       <c r="G401" s="1" t="s">
         <v>46</v>
       </c>
@@ -41247,6 +42435,9 @@
       <c r="E402" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F402" s="1">
+        <v>1679</v>
+      </c>
       <c r="G402" s="1" t="s">
         <v>46</v>
       </c>
@@ -41327,6 +42518,9 @@
       <c r="E403" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F403" s="1">
+        <v>1679</v>
+      </c>
       <c r="G403" s="1" t="s">
         <v>46</v>
       </c>
@@ -41407,6 +42601,9 @@
       <c r="E404" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="F404" s="1">
+        <v>1679</v>
+      </c>
       <c r="G404" s="1" t="s">
         <v>46</v>
       </c>
@@ -41496,6 +42693,9 @@
       <c r="E405" s="1" t="s">
         <v>1943</v>
       </c>
+      <c r="F405" s="1">
+        <v>1679</v>
+      </c>
       <c r="G405" s="1" t="s">
         <v>31</v>
       </c>
@@ -41585,6 +42785,9 @@
       <c r="E406" s="1" t="s">
         <v>1948</v>
       </c>
+      <c r="F406" s="1">
+        <v>1679</v>
+      </c>
       <c r="G406" s="1" t="s">
         <v>31</v>
       </c>
@@ -41671,6 +42874,9 @@
       <c r="E407" s="1" t="s">
         <v>1948</v>
       </c>
+      <c r="F407" s="1">
+        <v>1679</v>
+      </c>
       <c r="G407" s="1" t="s">
         <v>46</v>
       </c>
@@ -41757,6 +42963,9 @@
       <c r="E408" s="1" t="s">
         <v>1948</v>
       </c>
+      <c r="F408" s="1">
+        <v>1679</v>
+      </c>
       <c r="G408" s="1" t="s">
         <v>46</v>
       </c>
@@ -41843,6 +43052,9 @@
       <c r="E409" s="1" t="s">
         <v>1961</v>
       </c>
+      <c r="F409" s="1">
+        <v>1680</v>
+      </c>
       <c r="G409" s="1" t="s">
         <v>46</v>
       </c>
@@ -41932,6 +43144,9 @@
       <c r="E410" s="1" t="s">
         <v>1966</v>
       </c>
+      <c r="F410" s="1">
+        <v>1680</v>
+      </c>
       <c r="G410" s="1" t="s">
         <v>31</v>
       </c>
@@ -42006,6 +43221,9 @@
       <c r="E411" s="1" t="s">
         <v>1970</v>
       </c>
+      <c r="F411" s="1">
+        <v>1680</v>
+      </c>
       <c r="G411" s="1" t="s">
         <v>46</v>
       </c>
@@ -42095,6 +43313,9 @@
       <c r="E412" s="1" t="s">
         <v>1978</v>
       </c>
+      <c r="F412" s="1">
+        <v>1680</v>
+      </c>
       <c r="G412" s="1" t="s">
         <v>46</v>
       </c>
@@ -42181,6 +43402,9 @@
       <c r="E413" s="1" t="s">
         <v>1983</v>
       </c>
+      <c r="F413" s="1">
+        <v>1680</v>
+      </c>
       <c r="G413" s="1" t="s">
         <v>31</v>
       </c>
@@ -42267,6 +43491,9 @@
       <c r="E414" s="1" t="s">
         <v>1990</v>
       </c>
+      <c r="F414" s="1">
+        <v>1680</v>
+      </c>
       <c r="G414" s="1" t="s">
         <v>46</v>
       </c>
@@ -42353,6 +43580,9 @@
       <c r="E415" s="1" t="s">
         <v>1998</v>
       </c>
+      <c r="F415" s="1">
+        <v>1656</v>
+      </c>
       <c r="G415" s="1" t="s">
         <v>46</v>
       </c>
@@ -42439,6 +43669,9 @@
       <c r="E416" s="1" t="s">
         <v>2004</v>
       </c>
+      <c r="F416" s="1">
+        <v>1656</v>
+      </c>
       <c r="G416" s="1" t="s">
         <v>46</v>
       </c>
@@ -42525,6 +43758,9 @@
       <c r="E417" s="1" t="s">
         <v>2011</v>
       </c>
+      <c r="F417" s="1">
+        <v>1670</v>
+      </c>
       <c r="G417" s="1" t="s">
         <v>46</v>
       </c>
@@ -42614,6 +43850,9 @@
       <c r="E418" s="1" t="s">
         <v>2011</v>
       </c>
+      <c r="F418" s="1">
+        <v>1670</v>
+      </c>
       <c r="G418" s="1" t="s">
         <v>46</v>
       </c>
@@ -42694,6 +43933,9 @@
       <c r="E419" s="1" t="s">
         <v>2019</v>
       </c>
+      <c r="F419" s="1">
+        <v>1670</v>
+      </c>
       <c r="G419" s="1" t="s">
         <v>46</v>
       </c>
@@ -42782,6 +44024,9 @@
       </c>
       <c r="E420" s="1" t="s">
         <v>2019</v>
+      </c>
+      <c r="F420" s="1">
+        <v>1670</v>
       </c>
       <c r="G420" s="1" t="s">
         <v>46</v>

</xml_diff>